<commit_message>
Work on the final project
</commit_message>
<xml_diff>
--- a/projects/project-7-final/data/population.xlsx
+++ b/projects/project-7-final/data/population.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>region</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Пермский край</t>
   </si>
   <si>
-    <t>Коми-Пермяцкий округ, входящий в состав Пермского края</t>
-  </si>
-  <si>
     <t>Кировская область</t>
   </si>
   <si>
@@ -304,27 +301,15 @@
     <t>Алтайский край</t>
   </si>
   <si>
-    <t>Агинский Бурятский округ (Забайкальский край)</t>
-  </si>
-  <si>
     <t>Красноярский край</t>
   </si>
   <si>
-    <t>Таймырский (Долгано-Ненецкий) автономный округ (Красноярский край)</t>
-  </si>
-  <si>
-    <t>Эвенкийский автономный округ (Красноярский край)</t>
-  </si>
-  <si>
     <t>Иркутская область</t>
   </si>
   <si>
     <t>Кемеровская область - Кузбасс</t>
   </si>
   <si>
-    <t>Усть-Ордынский Бурятский округ</t>
-  </si>
-  <si>
     <t>Новосибирская область</t>
   </si>
   <si>
@@ -346,9 +331,6 @@
     <t>Камчатский край</t>
   </si>
   <si>
-    <t>Корякский округ, входящий в состав Камчатского края</t>
-  </si>
-  <si>
     <t>Приморский край</t>
   </si>
   <si>
@@ -368,9 +350,6 @@
   </si>
   <si>
     <t>Чукотский автономный округ</t>
-  </si>
-  <si>
-    <t>Крымский федеральный округ</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z189"/>
+  <dimension ref="A1:Z175"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7194,7 +7173,7 @@
       </c>
       <c r="Z105" s="4"/>
     </row>
-    <row r="106" ht="38.5" customHeight="1">
+    <row r="106" ht="14.5" customHeight="1">
       <c r="A106" t="s" s="2">
         <v>78</v>
       </c>
@@ -7229,37 +7208,77 @@
         <v>26</v>
       </c>
       <c r="B107" s="6">
-        <v>139790</v>
+        <v>1568722</v>
       </c>
       <c r="C107" s="6">
-        <v>138877</v>
+        <v>1553595</v>
       </c>
       <c r="D107" s="6">
-        <v>137648</v>
+        <v>1536772</v>
       </c>
       <c r="E107" s="6">
-        <v>136608</v>
-      </c>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
-      <c r="L107" s="5"/>
-      <c r="M107" s="5"/>
-      <c r="N107" s="5"/>
-      <c r="O107" s="5"/>
-      <c r="P107" s="5"/>
-      <c r="Q107" s="5"/>
-      <c r="R107" s="5"/>
-      <c r="S107" s="5"/>
-      <c r="T107" s="5"/>
-      <c r="U107" s="5"/>
-      <c r="V107" s="5"/>
-      <c r="W107" s="5"/>
-      <c r="X107" s="5"/>
-      <c r="Y107" s="5"/>
+        <v>1518378</v>
+      </c>
+      <c r="F107" s="6">
+        <v>1498976</v>
+      </c>
+      <c r="G107" s="6">
+        <v>1472481</v>
+      </c>
+      <c r="H107" s="6">
+        <v>1445356</v>
+      </c>
+      <c r="I107" s="6">
+        <v>1418645</v>
+      </c>
+      <c r="J107" s="6">
+        <v>1396017</v>
+      </c>
+      <c r="K107" s="6">
+        <v>1379383</v>
+      </c>
+      <c r="L107" s="6">
+        <v>1365003</v>
+      </c>
+      <c r="M107" s="6">
+        <v>1352692</v>
+      </c>
+      <c r="N107" s="6">
+        <v>1338758</v>
+      </c>
+      <c r="O107" s="6">
+        <v>1327915</v>
+      </c>
+      <c r="P107" s="6">
+        <v>1319076</v>
+      </c>
+      <c r="Q107" s="6">
+        <v>1310929</v>
+      </c>
+      <c r="R107" s="6">
+        <v>1304348</v>
+      </c>
+      <c r="S107" s="6">
+        <v>1297474</v>
+      </c>
+      <c r="T107" s="6">
+        <v>1291684</v>
+      </c>
+      <c r="U107" s="6">
+        <v>1283238</v>
+      </c>
+      <c r="V107" s="6">
+        <v>1272109</v>
+      </c>
+      <c r="W107" s="6">
+        <v>1262402</v>
+      </c>
+      <c r="X107" s="6">
+        <v>1250173</v>
+      </c>
+      <c r="Y107" s="6">
+        <v>1234780</v>
+      </c>
       <c r="Z107" s="4"/>
     </row>
     <row r="108" ht="14.5" customHeight="1">
@@ -7297,76 +7316,76 @@
         <v>26</v>
       </c>
       <c r="B109" s="6">
-        <v>1568722</v>
+        <v>3655489</v>
       </c>
       <c r="C109" s="6">
-        <v>1553595</v>
+        <v>3628222</v>
       </c>
       <c r="D109" s="6">
-        <v>1536772</v>
+        <v>3594476</v>
       </c>
       <c r="E109" s="6">
-        <v>1518378</v>
+        <v>3554696</v>
       </c>
       <c r="F109" s="6">
-        <v>1498976</v>
+        <v>3515673</v>
       </c>
       <c r="G109" s="6">
-        <v>1472481</v>
+        <v>3481080</v>
       </c>
       <c r="H109" s="6">
-        <v>1445356</v>
+        <v>3447896</v>
       </c>
       <c r="I109" s="6">
-        <v>1418645</v>
+        <v>3414325</v>
       </c>
       <c r="J109" s="6">
-        <v>1396017</v>
+        <v>3384358</v>
       </c>
       <c r="K109" s="6">
-        <v>1379383</v>
+        <v>3362817</v>
       </c>
       <c r="L109" s="6">
-        <v>1365003</v>
+        <v>3343719</v>
       </c>
       <c r="M109" s="6">
-        <v>1352692</v>
+        <v>3326812</v>
       </c>
       <c r="N109" s="6">
-        <v>1338758</v>
+        <v>3307648</v>
       </c>
       <c r="O109" s="6">
-        <v>1327915</v>
+        <v>3296947</v>
       </c>
       <c r="P109" s="6">
-        <v>1319076</v>
+        <v>3289841</v>
       </c>
       <c r="Q109" s="6">
-        <v>1310929</v>
+        <v>3281496</v>
       </c>
       <c r="R109" s="6">
-        <v>1304348</v>
+        <v>3270203</v>
       </c>
       <c r="S109" s="6">
-        <v>1297474</v>
+        <v>3260267</v>
       </c>
       <c r="T109" s="6">
-        <v>1291684</v>
+        <v>3247713</v>
       </c>
       <c r="U109" s="6">
-        <v>1283238</v>
+        <v>3234752</v>
       </c>
       <c r="V109" s="6">
-        <v>1272109</v>
+        <v>3214623</v>
       </c>
       <c r="W109" s="6">
-        <v>1262402</v>
+        <v>3202946</v>
       </c>
       <c r="X109" s="6">
-        <v>1250173</v>
+        <v>3176552</v>
       </c>
       <c r="Y109" s="6">
-        <v>1234780</v>
+        <v>3144254</v>
       </c>
       <c r="Z109" s="4"/>
     </row>
@@ -7405,76 +7424,76 @@
         <v>26</v>
       </c>
       <c r="B111" s="6">
-        <v>3655489</v>
+        <v>2217558</v>
       </c>
       <c r="C111" s="6">
-        <v>3628222</v>
+        <v>2211204</v>
       </c>
       <c r="D111" s="6">
-        <v>3594476</v>
+        <v>2203616</v>
       </c>
       <c r="E111" s="6">
-        <v>3554696</v>
+        <v>2189876</v>
       </c>
       <c r="F111" s="6">
-        <v>3515673</v>
+        <v>2176000</v>
       </c>
       <c r="G111" s="6">
-        <v>3481080</v>
+        <v>2149942</v>
       </c>
       <c r="H111" s="6">
-        <v>3447896</v>
+        <v>2122459</v>
       </c>
       <c r="I111" s="6">
-        <v>3414325</v>
+        <v>2093495</v>
       </c>
       <c r="J111" s="6">
-        <v>3384358</v>
+        <v>2067890</v>
       </c>
       <c r="K111" s="6">
-        <v>3362817</v>
+        <v>2055701</v>
       </c>
       <c r="L111" s="6">
-        <v>3343719</v>
+        <v>2044256</v>
       </c>
       <c r="M111" s="6">
-        <v>3326812</v>
+        <v>2042043</v>
       </c>
       <c r="N111" s="6">
-        <v>3307648</v>
+        <v>2031497</v>
       </c>
       <c r="O111" s="6">
-        <v>3296947</v>
+        <v>2023665</v>
       </c>
       <c r="P111" s="6">
-        <v>3289841</v>
+        <v>2016086</v>
       </c>
       <c r="Q111" s="6">
-        <v>3281496</v>
+        <v>2008566</v>
       </c>
       <c r="R111" s="6">
-        <v>3270203</v>
+        <v>2001110</v>
       </c>
       <c r="S111" s="6">
-        <v>3260267</v>
+        <v>1994762</v>
       </c>
       <c r="T111" s="6">
-        <v>3247713</v>
+        <v>1989589</v>
       </c>
       <c r="U111" s="6">
-        <v>3234752</v>
+        <v>1977720</v>
       </c>
       <c r="V111" s="6">
-        <v>3214623</v>
+        <v>1963007</v>
       </c>
       <c r="W111" s="6">
-        <v>3202946</v>
+        <v>1956835</v>
       </c>
       <c r="X111" s="6">
-        <v>3176552</v>
+        <v>1942915</v>
       </c>
       <c r="Y111" s="6">
-        <v>3144254</v>
+        <v>1924578</v>
       </c>
       <c r="Z111" s="4"/>
     </row>
@@ -7513,76 +7532,76 @@
         <v>26</v>
       </c>
       <c r="B113" s="6">
-        <v>2217558</v>
+        <v>1514283</v>
       </c>
       <c r="C113" s="6">
-        <v>2211204</v>
+        <v>1500196</v>
       </c>
       <c r="D113" s="6">
-        <v>2203616</v>
+        <v>1484149</v>
       </c>
       <c r="E113" s="6">
-        <v>2189876</v>
+        <v>1466215</v>
       </c>
       <c r="F113" s="6">
-        <v>2176000</v>
+        <v>1449233</v>
       </c>
       <c r="G113" s="6">
-        <v>2149942</v>
+        <v>1439986</v>
       </c>
       <c r="H113" s="6">
-        <v>2122459</v>
+        <v>1431060</v>
       </c>
       <c r="I113" s="6">
-        <v>2093495</v>
+        <v>1420065</v>
       </c>
       <c r="J113" s="6">
-        <v>2067890</v>
+        <v>1411733</v>
       </c>
       <c r="K113" s="6">
-        <v>2055701</v>
+        <v>1405351</v>
       </c>
       <c r="L113" s="6">
-        <v>2044256</v>
+        <v>1398160</v>
       </c>
       <c r="M113" s="6">
-        <v>2042043</v>
+        <v>1392414</v>
       </c>
       <c r="N113" s="6">
-        <v>2031497</v>
+        <v>1384006</v>
       </c>
       <c r="O113" s="6">
-        <v>2023665</v>
+        <v>1376538</v>
       </c>
       <c r="P113" s="6">
-        <v>2016086</v>
+        <v>1368657</v>
       </c>
       <c r="Q113" s="6">
-        <v>2008566</v>
+        <v>1360587</v>
       </c>
       <c r="R113" s="6">
-        <v>2001110</v>
+        <v>1355618</v>
       </c>
       <c r="S113" s="6">
-        <v>1994762</v>
+        <v>1348703</v>
       </c>
       <c r="T113" s="6">
-        <v>1989589</v>
+        <v>1341526</v>
       </c>
       <c r="U113" s="6">
-        <v>1977720</v>
+        <v>1331655</v>
       </c>
       <c r="V113" s="6">
-        <v>1963007</v>
+        <v>1318103</v>
       </c>
       <c r="W113" s="6">
-        <v>1956835</v>
+        <v>1305563</v>
       </c>
       <c r="X113" s="6">
-        <v>1942915</v>
+        <v>1290898</v>
       </c>
       <c r="Y113" s="6">
-        <v>1924578</v>
+        <v>1274062</v>
       </c>
       <c r="Z113" s="4"/>
     </row>
@@ -7621,76 +7640,76 @@
         <v>26</v>
       </c>
       <c r="B115" s="6">
-        <v>1514283</v>
+        <v>3302566</v>
       </c>
       <c r="C115" s="6">
-        <v>1500196</v>
+        <v>3291598</v>
       </c>
       <c r="D115" s="6">
-        <v>1484149</v>
+        <v>3275823</v>
       </c>
       <c r="E115" s="6">
-        <v>1466215</v>
+        <v>3254055</v>
       </c>
       <c r="F115" s="6">
-        <v>1449233</v>
+        <v>3235699</v>
       </c>
       <c r="G115" s="6">
-        <v>1439986</v>
+        <v>3229151</v>
       </c>
       <c r="H115" s="6">
-        <v>1431060</v>
+        <v>3225275</v>
       </c>
       <c r="I115" s="6">
-        <v>1420065</v>
+        <v>3225643</v>
       </c>
       <c r="J115" s="6">
-        <v>1411733</v>
+        <v>3223938</v>
       </c>
       <c r="K115" s="6">
-        <v>1405351</v>
+        <v>3220938</v>
       </c>
       <c r="L115" s="6">
-        <v>1398160</v>
+        <v>3221513</v>
       </c>
       <c r="M115" s="6">
-        <v>1392414</v>
+        <v>3220910</v>
       </c>
       <c r="N115" s="6">
-        <v>1384006</v>
+        <v>3215311</v>
       </c>
       <c r="O115" s="6">
-        <v>1376538</v>
+        <v>3214065</v>
       </c>
       <c r="P115" s="6">
-        <v>1368657</v>
+        <v>3213289</v>
       </c>
       <c r="Q115" s="6">
-        <v>1360587</v>
+        <v>3211187</v>
       </c>
       <c r="R115" s="6">
-        <v>1355618</v>
+        <v>3212676</v>
       </c>
       <c r="S115" s="6">
-        <v>1348703</v>
+        <v>3205975</v>
       </c>
       <c r="T115" s="6">
-        <v>1341526</v>
+        <v>3203679</v>
       </c>
       <c r="U115" s="6">
-        <v>1331655</v>
+        <v>3193514</v>
       </c>
       <c r="V115" s="6">
-        <v>1318103</v>
+        <v>3183038</v>
       </c>
       <c r="W115" s="6">
-        <v>1305563</v>
+        <v>3179532</v>
       </c>
       <c r="X115" s="6">
-        <v>1290898</v>
+        <v>3154164</v>
       </c>
       <c r="Y115" s="6">
-        <v>1274062</v>
+        <v>3131720</v>
       </c>
       <c r="Z115" s="4"/>
     </row>
@@ -7729,76 +7748,76 @@
         <v>26</v>
       </c>
       <c r="B117" s="6">
-        <v>3302566</v>
+        <v>2719990</v>
       </c>
       <c r="C117" s="6">
-        <v>3291598</v>
+        <v>2710645</v>
       </c>
       <c r="D117" s="6">
-        <v>3275823</v>
+        <v>2699385</v>
       </c>
       <c r="E117" s="6">
-        <v>3254055</v>
+        <v>2682054</v>
       </c>
       <c r="F117" s="6">
-        <v>3235699</v>
+        <v>2663481</v>
       </c>
       <c r="G117" s="6">
-        <v>3229151</v>
+        <v>2639528</v>
       </c>
       <c r="H117" s="6">
-        <v>3225275</v>
+        <v>2615575</v>
       </c>
       <c r="I117" s="6">
-        <v>3225643</v>
+        <v>2591231</v>
       </c>
       <c r="J117" s="6">
-        <v>3223938</v>
+        <v>2572396</v>
       </c>
       <c r="K117" s="6">
-        <v>3220938</v>
+        <v>2558322</v>
       </c>
       <c r="L117" s="6">
-        <v>3221513</v>
+        <v>2545296</v>
       </c>
       <c r="M117" s="6">
-        <v>3220910</v>
+        <v>2535434</v>
       </c>
       <c r="N117" s="6">
-        <v>3215311</v>
+        <v>2519282</v>
       </c>
       <c r="O117" s="6">
-        <v>3214065</v>
+        <v>2508754</v>
       </c>
       <c r="P117" s="6">
-        <v>3213289</v>
+        <v>2503305</v>
       </c>
       <c r="Q117" s="6">
-        <v>3211187</v>
+        <v>2496552</v>
       </c>
       <c r="R117" s="6">
-        <v>3212676</v>
+        <v>2493024</v>
       </c>
       <c r="S117" s="6">
-        <v>3205975</v>
+        <v>2487529</v>
       </c>
       <c r="T117" s="6">
-        <v>3203679</v>
+        <v>2479260</v>
       </c>
       <c r="U117" s="6">
-        <v>3193514</v>
+        <v>2462950</v>
       </c>
       <c r="V117" s="6">
-        <v>3183038</v>
+        <v>2440815</v>
       </c>
       <c r="W117" s="6">
-        <v>3179532</v>
+        <v>2421895</v>
       </c>
       <c r="X117" s="6">
-        <v>3154164</v>
+        <v>2395111</v>
       </c>
       <c r="Y117" s="6">
-        <v>3131720</v>
+        <v>2360959</v>
       </c>
       <c r="Z117" s="4"/>
     </row>
@@ -7837,76 +7856,76 @@
         <v>26</v>
       </c>
       <c r="B119" s="6">
-        <v>2719990</v>
+        <v>1439759</v>
       </c>
       <c r="C119" s="6">
-        <v>2710645</v>
+        <v>1427375</v>
       </c>
       <c r="D119" s="6">
-        <v>2699385</v>
+        <v>1413571</v>
       </c>
       <c r="E119" s="6">
-        <v>2682054</v>
+        <v>1395882</v>
       </c>
       <c r="F119" s="6">
-        <v>2663481</v>
+        <v>1378931</v>
       </c>
       <c r="G119" s="6">
-        <v>2639528</v>
+        <v>1366879</v>
       </c>
       <c r="H119" s="6">
-        <v>2615575</v>
+        <v>1354580</v>
       </c>
       <c r="I119" s="6">
-        <v>2591231</v>
+        <v>1340335</v>
       </c>
       <c r="J119" s="6">
-        <v>2572396</v>
+        <v>1325914</v>
       </c>
       <c r="K119" s="6">
-        <v>2558322</v>
+        <v>1316217</v>
       </c>
       <c r="L119" s="6">
-        <v>2545296</v>
+        <v>1308692</v>
       </c>
       <c r="M119" s="6">
-        <v>2535434</v>
+        <v>1301689</v>
       </c>
       <c r="N119" s="6">
-        <v>2519282</v>
+        <v>1290478</v>
       </c>
       <c r="O119" s="6">
-        <v>2508754</v>
+        <v>1282094</v>
       </c>
       <c r="P119" s="6">
-        <v>2503305</v>
+        <v>1274487</v>
       </c>
       <c r="Q119" s="6">
-        <v>2496552</v>
+        <v>1267561</v>
       </c>
       <c r="R119" s="6">
-        <v>2493024</v>
+        <v>1262549</v>
       </c>
       <c r="S119" s="6">
-        <v>2487529</v>
+        <v>1257621</v>
       </c>
       <c r="T119" s="6">
-        <v>2479260</v>
+        <v>1252887</v>
       </c>
       <c r="U119" s="6">
-        <v>2462950</v>
+        <v>1246618</v>
       </c>
       <c r="V119" s="6">
-        <v>2440815</v>
+        <v>1238416</v>
       </c>
       <c r="W119" s="6">
-        <v>2421895</v>
+        <v>1229824</v>
       </c>
       <c r="X119" s="6">
-        <v>2395111</v>
+        <v>1218319</v>
       </c>
       <c r="Y119" s="6">
-        <v>2360959</v>
+        <v>1203969</v>
       </c>
       <c r="Z119" s="4"/>
     </row>
@@ -7945,76 +7964,76 @@
         <v>26</v>
       </c>
       <c r="B121" s="6">
-        <v>1439759</v>
+        <v>1068503</v>
       </c>
       <c r="C121" s="6">
-        <v>1427375</v>
+        <v>1059515</v>
       </c>
       <c r="D121" s="6">
-        <v>1413571</v>
+        <v>1047114</v>
       </c>
       <c r="E121" s="6">
-        <v>1395882</v>
+        <v>1030748</v>
       </c>
       <c r="F121" s="6">
-        <v>1378931</v>
+        <v>1016184</v>
       </c>
       <c r="G121" s="6">
-        <v>1366879</v>
+        <v>999446</v>
       </c>
       <c r="H121" s="6">
-        <v>1354580</v>
+        <v>981029</v>
       </c>
       <c r="I121" s="6">
-        <v>1340335</v>
+        <v>961815</v>
       </c>
       <c r="J121" s="6">
-        <v>1325914</v>
+        <v>946068</v>
       </c>
       <c r="K121" s="6">
-        <v>1316217</v>
+        <v>934512</v>
       </c>
       <c r="L121" s="6">
-        <v>1308692</v>
+        <v>925180</v>
       </c>
       <c r="M121" s="6">
-        <v>1301689</v>
+        <v>918585</v>
       </c>
       <c r="N121" s="6">
-        <v>1290478</v>
+        <v>908813</v>
       </c>
       <c r="O121" s="6">
-        <v>1282094</v>
+        <v>896264</v>
       </c>
       <c r="P121" s="6">
-        <v>1274487</v>
+        <v>885759</v>
       </c>
       <c r="Q121" s="6">
-        <v>1267561</v>
+        <v>877149</v>
       </c>
       <c r="R121" s="6">
-        <v>1262549</v>
+        <v>869814</v>
       </c>
       <c r="S121" s="6">
-        <v>1257621</v>
+        <v>861896</v>
       </c>
       <c r="T121" s="6">
-        <v>1252887</v>
+        <v>854109</v>
       </c>
       <c r="U121" s="6">
-        <v>1246618</v>
+        <v>845537</v>
       </c>
       <c r="V121" s="6">
-        <v>1238416</v>
+        <v>834701</v>
       </c>
       <c r="W121" s="6">
-        <v>1229824</v>
+        <v>827166</v>
       </c>
       <c r="X121" s="6">
-        <v>1218319</v>
+        <v>818570</v>
       </c>
       <c r="Y121" s="6">
-        <v>1203969</v>
+        <v>805510</v>
       </c>
       <c r="Z121" s="4"/>
     </row>
@@ -8053,76 +8072,76 @@
         <v>26</v>
       </c>
       <c r="B123" s="6">
-        <v>1068503</v>
+        <v>4607587</v>
       </c>
       <c r="C123" s="6">
-        <v>1059515</v>
+        <v>4577515</v>
       </c>
       <c r="D123" s="6">
-        <v>1047114</v>
+        <v>4545942</v>
       </c>
       <c r="E123" s="6">
-        <v>1030748</v>
+        <v>4514084</v>
       </c>
       <c r="F123" s="6">
-        <v>1016184</v>
+        <v>4477552</v>
       </c>
       <c r="G123" s="6">
-        <v>999446</v>
+        <v>4434165</v>
       </c>
       <c r="H123" s="6">
-        <v>981029</v>
+        <v>4394041</v>
       </c>
       <c r="I123" s="6">
-        <v>961815</v>
+        <v>4356425</v>
       </c>
       <c r="J123" s="6">
-        <v>946068</v>
+        <v>4330579</v>
       </c>
       <c r="K123" s="6">
-        <v>934512</v>
+        <v>4320114</v>
       </c>
       <c r="L123" s="6">
-        <v>925180</v>
+        <v>4314337</v>
       </c>
       <c r="M123" s="6">
-        <v>918585</v>
+        <v>4308472</v>
       </c>
       <c r="N123" s="6">
-        <v>908813</v>
+        <v>4297227</v>
       </c>
       <c r="O123" s="6">
-        <v>896264</v>
+        <v>4307594</v>
       </c>
       <c r="P123" s="6">
-        <v>885759</v>
+        <v>4315830</v>
       </c>
       <c r="Q123" s="6">
-        <v>877149</v>
+        <v>4320677</v>
       </c>
       <c r="R123" s="6">
-        <v>869814</v>
+        <v>4327472</v>
       </c>
       <c r="S123" s="6">
-        <v>861896</v>
+        <v>4330006</v>
       </c>
       <c r="T123" s="6">
-        <v>854109</v>
+        <v>4329341</v>
       </c>
       <c r="U123" s="6">
-        <v>845537</v>
+        <v>4325256</v>
       </c>
       <c r="V123" s="6">
-        <v>834701</v>
+        <v>4315699</v>
       </c>
       <c r="W123" s="6">
-        <v>827166</v>
+        <v>4310681</v>
       </c>
       <c r="X123" s="6">
-        <v>818570</v>
+        <v>4290067</v>
       </c>
       <c r="Y123" s="6">
-        <v>805510</v>
+        <v>4264340</v>
       </c>
       <c r="Z123" s="4"/>
     </row>
@@ -8161,80 +8180,80 @@
         <v>26</v>
       </c>
       <c r="B125" s="6">
-        <v>4607587</v>
+        <v>3226093</v>
       </c>
       <c r="C125" s="6">
-        <v>4577515</v>
+        <v>3218356</v>
       </c>
       <c r="D125" s="6">
-        <v>4545942</v>
+        <v>3234252</v>
       </c>
       <c r="E125" s="6">
-        <v>4514084</v>
+        <v>3251484</v>
       </c>
       <c r="F125" s="6">
-        <v>4477552</v>
+        <v>3269862</v>
       </c>
       <c r="G125" s="6">
-        <v>4434165</v>
+        <v>3281655</v>
       </c>
       <c r="H125" s="6">
-        <v>4394041</v>
+        <v>3288337</v>
       </c>
       <c r="I125" s="6">
-        <v>4356425</v>
+        <v>3293830</v>
       </c>
       <c r="J125" s="6">
-        <v>4330579</v>
+        <v>3306698</v>
       </c>
       <c r="K125" s="6">
-        <v>4320114</v>
+        <v>3330607</v>
       </c>
       <c r="L125" s="6">
-        <v>4314337</v>
+        <v>3351694</v>
       </c>
       <c r="M125" s="6">
-        <v>4308472</v>
+        <v>3378795</v>
       </c>
       <c r="N125" s="6">
-        <v>4297227</v>
+        <v>3405265</v>
       </c>
       <c r="O125" s="6">
-        <v>4307594</v>
+        <v>3459438</v>
       </c>
       <c r="P125" s="6">
-        <v>4315830</v>
+        <v>3510683</v>
       </c>
       <c r="Q125" s="6">
-        <v>4320677</v>
+        <v>3546345</v>
       </c>
       <c r="R125" s="6">
-        <v>4327472</v>
+        <v>3581293</v>
       </c>
       <c r="S125" s="6">
-        <v>4330006</v>
+        <v>3615485</v>
       </c>
       <c r="T125" s="6">
-        <v>4329341</v>
+        <v>3660030</v>
       </c>
       <c r="U125" s="6">
-        <v>4325256</v>
+        <v>3692400</v>
       </c>
       <c r="V125" s="6">
-        <v>4315699</v>
+        <v>3723969</v>
       </c>
       <c r="W125" s="6">
-        <v>4310681</v>
+        <v>3756536</v>
       </c>
       <c r="X125" s="6">
-        <v>4290067</v>
+        <v>3778053</v>
       </c>
       <c r="Y125" s="6">
-        <v>4264340</v>
+        <v>3806505</v>
       </c>
       <c r="Z125" s="4"/>
     </row>
-    <row r="126" ht="14.5" customHeight="1">
+    <row r="126" ht="38.5" customHeight="1">
       <c r="A126" t="s" s="2">
         <v>88</v>
       </c>
@@ -8269,80 +8288,80 @@
         <v>26</v>
       </c>
       <c r="B127" s="6">
-        <v>3226093</v>
+        <v>1359069</v>
       </c>
       <c r="C127" s="6">
-        <v>3218356</v>
+        <v>1359646</v>
       </c>
       <c r="D127" s="6">
-        <v>3234252</v>
+        <v>1383449</v>
       </c>
       <c r="E127" s="6">
-        <v>3251484</v>
+        <v>1411867</v>
       </c>
       <c r="F127" s="6">
-        <v>3269862</v>
+        <v>1437729</v>
       </c>
       <c r="G127" s="6">
-        <v>3281655</v>
+        <v>1453541</v>
       </c>
       <c r="H127" s="6">
-        <v>3288337</v>
+        <v>1462194</v>
       </c>
       <c r="I127" s="6">
-        <v>3293830</v>
+        <v>1467792</v>
       </c>
       <c r="J127" s="6">
-        <v>3306698</v>
+        <v>1475188</v>
       </c>
       <c r="K127" s="6">
-        <v>3330607</v>
+        <v>1491240</v>
       </c>
       <c r="L127" s="6">
-        <v>3351694</v>
+        <v>1504319</v>
       </c>
       <c r="M127" s="6">
-        <v>3378795</v>
+        <v>1521222</v>
       </c>
       <c r="N127" s="6">
-        <v>3405265</v>
+        <v>1537134</v>
       </c>
       <c r="O127" s="6">
-        <v>3459438</v>
+        <v>1561238</v>
       </c>
       <c r="P127" s="6">
-        <v>3510683</v>
+        <v>1584063</v>
       </c>
       <c r="Q127" s="6">
-        <v>3546345</v>
+        <v>1597248</v>
       </c>
       <c r="R127" s="6">
-        <v>3581293</v>
+        <v>1612076</v>
       </c>
       <c r="S127" s="6">
-        <v>3615485</v>
+        <v>1626755</v>
       </c>
       <c r="T127" s="6">
-        <v>3660030</v>
+        <v>1646078</v>
       </c>
       <c r="U127" s="6">
-        <v>3692400</v>
+        <v>1655074</v>
       </c>
       <c r="V127" s="6">
-        <v>3723969</v>
+        <v>1663795</v>
       </c>
       <c r="W127" s="6">
-        <v>3756536</v>
+        <v>1674676</v>
       </c>
       <c r="X127" s="6">
-        <v>3778053</v>
+        <v>1687654</v>
       </c>
       <c r="Y127" s="6">
-        <v>3806505</v>
+        <v>1702240</v>
       </c>
       <c r="Z127" s="4"/>
     </row>
-    <row r="128" ht="38.5" customHeight="1">
+    <row r="128" ht="26.5" customHeight="1">
       <c r="A128" t="s" s="2">
         <v>89</v>
       </c>
@@ -8377,80 +8396,80 @@
         <v>26</v>
       </c>
       <c r="B129" s="6">
-        <v>1359069</v>
+        <v>498996</v>
       </c>
       <c r="C129" s="6">
-        <v>1359646</v>
+        <v>496292</v>
       </c>
       <c r="D129" s="6">
-        <v>1383449</v>
+        <v>498271</v>
       </c>
       <c r="E129" s="6">
-        <v>1411867</v>
+        <v>503121</v>
       </c>
       <c r="F129" s="6">
-        <v>1437729</v>
+        <v>508600</v>
       </c>
       <c r="G129" s="6">
-        <v>1453541</v>
+        <v>510846</v>
       </c>
       <c r="H129" s="6">
-        <v>1462194</v>
+        <v>514581</v>
       </c>
       <c r="I129" s="6">
-        <v>1467792</v>
+        <v>517385</v>
       </c>
       <c r="J129" s="6">
-        <v>1475188</v>
+        <v>521621</v>
       </c>
       <c r="K129" s="6">
-        <v>1491240</v>
+        <v>524012</v>
       </c>
       <c r="L129" s="6">
-        <v>1504319</v>
+        <v>522966</v>
       </c>
       <c r="M129" s="6">
-        <v>1521222</v>
+        <v>524141</v>
       </c>
       <c r="N129" s="6">
-        <v>1537134</v>
+        <v>524925</v>
       </c>
       <c r="O129" s="6">
-        <v>1561238</v>
+        <v>536558</v>
       </c>
       <c r="P129" s="6">
-        <v>1584063</v>
+        <v>541612</v>
       </c>
       <c r="Q129" s="6">
-        <v>1597248</v>
+        <v>539671</v>
       </c>
       <c r="R129" s="6">
-        <v>1612076</v>
+        <v>539985</v>
       </c>
       <c r="S129" s="6">
-        <v>1626755</v>
+        <v>534104</v>
       </c>
       <c r="T129" s="6">
-        <v>1646078</v>
+        <v>536049</v>
       </c>
       <c r="U129" s="6">
-        <v>1655074</v>
+        <v>538547</v>
       </c>
       <c r="V129" s="6">
-        <v>1663795</v>
+        <v>541479</v>
       </c>
       <c r="W129" s="6">
-        <v>1674676</v>
+        <v>544444</v>
       </c>
       <c r="X129" s="6">
-        <v>1687654</v>
+        <v>547010</v>
       </c>
       <c r="Y129" s="6">
-        <v>1702240</v>
+        <v>552117</v>
       </c>
       <c r="Z129" s="4"/>
     </row>
-    <row r="130" ht="26.5" customHeight="1">
+    <row r="130" ht="50.5" customHeight="1">
       <c r="A130" t="s" s="2">
         <v>90</v>
       </c>
@@ -8484,81 +8503,71 @@
       <c r="A131" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B131" s="6">
-        <v>498996</v>
-      </c>
-      <c r="C131" s="6">
-        <v>496292</v>
-      </c>
-      <c r="D131" s="6">
-        <v>498271</v>
-      </c>
-      <c r="E131" s="6">
-        <v>503121</v>
-      </c>
-      <c r="F131" s="6">
-        <v>508600</v>
-      </c>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
       <c r="G131" s="6">
-        <v>510846</v>
+        <v>1317268</v>
       </c>
       <c r="H131" s="6">
-        <v>514581</v>
+        <v>1311562</v>
       </c>
       <c r="I131" s="6">
-        <v>517385</v>
+        <v>1308653</v>
       </c>
       <c r="J131" s="6">
-        <v>521621</v>
+        <v>1309889</v>
       </c>
       <c r="K131" s="6">
-        <v>524012</v>
+        <v>1315355</v>
       </c>
       <c r="L131" s="6">
-        <v>522966</v>
+        <v>1324409</v>
       </c>
       <c r="M131" s="6">
-        <v>524141</v>
+        <v>1333432</v>
       </c>
       <c r="N131" s="6">
-        <v>524925</v>
+        <v>1343206</v>
       </c>
       <c r="O131" s="6">
-        <v>536558</v>
+        <v>1361642</v>
       </c>
       <c r="P131" s="6">
-        <v>541612</v>
+        <v>1385008</v>
       </c>
       <c r="Q131" s="6">
-        <v>539671</v>
+        <v>1409426</v>
       </c>
       <c r="R131" s="6">
-        <v>539985</v>
+        <v>1429232</v>
       </c>
       <c r="S131" s="6">
-        <v>534104</v>
+        <v>1454626</v>
       </c>
       <c r="T131" s="6">
-        <v>536049</v>
+        <v>1477903</v>
       </c>
       <c r="U131" s="6">
-        <v>538547</v>
+        <v>1498779</v>
       </c>
       <c r="V131" s="6">
-        <v>541479</v>
+        <v>1518695</v>
       </c>
       <c r="W131" s="6">
-        <v>544444</v>
+        <v>1537416</v>
       </c>
       <c r="X131" s="6">
-        <v>547010</v>
+        <v>1543389</v>
       </c>
       <c r="Y131" s="6">
-        <v>552117</v>
+        <v>1552148</v>
       </c>
       <c r="Z131" s="4"/>
     </row>
-    <row r="132" ht="50.5" customHeight="1">
+    <row r="132" ht="14.5" customHeight="1">
       <c r="A132" t="s" s="2">
         <v>91</v>
       </c>
@@ -8592,67 +8601,77 @@
       <c r="A133" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
+      <c r="B133" s="6">
+        <v>3671985</v>
+      </c>
+      <c r="C133" s="6">
+        <v>3660112</v>
+      </c>
+      <c r="D133" s="6">
+        <v>3643949</v>
+      </c>
+      <c r="E133" s="6">
+        <v>3621426</v>
+      </c>
+      <c r="F133" s="6">
+        <v>3597659</v>
+      </c>
       <c r="G133" s="6">
-        <v>1317268</v>
+        <v>3569284</v>
       </c>
       <c r="H133" s="6">
-        <v>1311562</v>
+        <v>3541787</v>
       </c>
       <c r="I133" s="6">
-        <v>1308653</v>
+        <v>3516661</v>
       </c>
       <c r="J133" s="6">
-        <v>1309889</v>
+        <v>3496983</v>
       </c>
       <c r="K133" s="6">
-        <v>1315355</v>
+        <v>3489092</v>
       </c>
       <c r="L133" s="6">
-        <v>1324409</v>
+        <v>3484809</v>
       </c>
       <c r="M133" s="6">
-        <v>1333432</v>
+        <v>3481818</v>
       </c>
       <c r="N133" s="6">
-        <v>1343206</v>
+        <v>3475634</v>
       </c>
       <c r="O133" s="6">
-        <v>1361642</v>
+        <v>3480142</v>
       </c>
       <c r="P133" s="6">
-        <v>1385008</v>
+        <v>3485272</v>
       </c>
       <c r="Q133" s="6">
-        <v>1409426</v>
+        <v>3490053</v>
       </c>
       <c r="R133" s="6">
-        <v>1429232</v>
+        <v>3497274</v>
       </c>
       <c r="S133" s="6">
-        <v>1454626</v>
+        <v>3500716</v>
       </c>
       <c r="T133" s="6">
-        <v>1477903</v>
+        <v>3502323</v>
       </c>
       <c r="U133" s="6">
-        <v>1498779</v>
+        <v>3493036</v>
       </c>
       <c r="V133" s="6">
-        <v>1518695</v>
+        <v>3475753</v>
       </c>
       <c r="W133" s="6">
-        <v>1537416</v>
+        <v>3466369</v>
       </c>
       <c r="X133" s="6">
-        <v>1543389</v>
+        <v>3442810</v>
       </c>
       <c r="Y133" s="6">
-        <v>1552148</v>
+        <v>3418606</v>
       </c>
       <c r="Z133" s="4"/>
     </row>
@@ -8691,76 +8710,76 @@
         <v>26</v>
       </c>
       <c r="B135" s="6">
-        <v>3671985</v>
+        <v>201699</v>
       </c>
       <c r="C135" s="6">
-        <v>3660112</v>
+        <v>202441</v>
       </c>
       <c r="D135" s="6">
-        <v>3643949</v>
+        <v>203030</v>
       </c>
       <c r="E135" s="6">
-        <v>3621426</v>
+        <v>202945</v>
       </c>
       <c r="F135" s="6">
-        <v>3597659</v>
+        <v>203038</v>
       </c>
       <c r="G135" s="6">
-        <v>3569284</v>
+        <v>202571</v>
       </c>
       <c r="H135" s="6">
-        <v>3541787</v>
+        <v>202333</v>
       </c>
       <c r="I135" s="6">
-        <v>3516661</v>
+        <v>201674</v>
       </c>
       <c r="J135" s="6">
-        <v>3496983</v>
+        <v>201744</v>
       </c>
       <c r="K135" s="6">
-        <v>3489092</v>
+        <v>203128</v>
       </c>
       <c r="L135" s="6">
-        <v>3484809</v>
+        <v>204687</v>
       </c>
       <c r="M135" s="6">
-        <v>3481818</v>
+        <v>205386</v>
       </c>
       <c r="N135" s="6">
-        <v>3475634</v>
+        <v>206530</v>
       </c>
       <c r="O135" s="6">
-        <v>3480142</v>
+        <v>208425</v>
       </c>
       <c r="P135" s="6">
-        <v>3485272</v>
+        <v>210344</v>
       </c>
       <c r="Q135" s="6">
-        <v>3490053</v>
+        <v>211645</v>
       </c>
       <c r="R135" s="6">
-        <v>3497274</v>
+        <v>213703</v>
       </c>
       <c r="S135" s="6">
-        <v>3500716</v>
+        <v>215161</v>
       </c>
       <c r="T135" s="6">
-        <v>3502323</v>
+        <v>217007</v>
       </c>
       <c r="U135" s="6">
-        <v>3493036</v>
+        <v>218063</v>
       </c>
       <c r="V135" s="6">
-        <v>3475753</v>
+        <v>218866</v>
       </c>
       <c r="W135" s="6">
-        <v>3466369</v>
+        <v>220181</v>
       </c>
       <c r="X135" s="6">
-        <v>3442810</v>
+        <v>220954</v>
       </c>
       <c r="Y135" s="6">
-        <v>3418606</v>
+        <v>221559</v>
       </c>
       <c r="Z135" s="4"/>
     </row>
@@ -8799,76 +8818,76 @@
         <v>26</v>
       </c>
       <c r="B137" s="6">
-        <v>201699</v>
+        <v>306169</v>
       </c>
       <c r="C137" s="6">
-        <v>202441</v>
+        <v>306152</v>
       </c>
       <c r="D137" s="6">
-        <v>203030</v>
+        <v>305729</v>
       </c>
       <c r="E137" s="6">
-        <v>202945</v>
+        <v>305216</v>
       </c>
       <c r="F137" s="6">
-        <v>203038</v>
+        <v>305493</v>
       </c>
       <c r="G137" s="6">
-        <v>202571</v>
+        <v>304957</v>
       </c>
       <c r="H137" s="6">
-        <v>202333</v>
+        <v>304066</v>
       </c>
       <c r="I137" s="6">
-        <v>201674</v>
+        <v>302889</v>
       </c>
       <c r="J137" s="6">
-        <v>201744</v>
+        <v>302357</v>
       </c>
       <c r="K137" s="6">
-        <v>203128</v>
+        <v>303783</v>
       </c>
       <c r="L137" s="6">
-        <v>204687</v>
+        <v>305306</v>
       </c>
       <c r="M137" s="6">
-        <v>205386</v>
+        <v>307323</v>
       </c>
       <c r="N137" s="6">
-        <v>206530</v>
+        <v>308132</v>
       </c>
       <c r="O137" s="6">
-        <v>208425</v>
+        <v>309347</v>
       </c>
       <c r="P137" s="6">
-        <v>210344</v>
+        <v>310460</v>
       </c>
       <c r="Q137" s="6">
-        <v>211645</v>
+        <v>311761</v>
       </c>
       <c r="R137" s="6">
-        <v>213703</v>
+        <v>313777</v>
       </c>
       <c r="S137" s="6">
-        <v>215161</v>
+        <v>315637</v>
       </c>
       <c r="T137" s="6">
-        <v>217007</v>
+        <v>318550</v>
       </c>
       <c r="U137" s="6">
-        <v>218063</v>
+        <v>321722</v>
       </c>
       <c r="V137" s="6">
-        <v>218866</v>
+        <v>324423</v>
       </c>
       <c r="W137" s="6">
-        <v>220181</v>
+        <v>327383</v>
       </c>
       <c r="X137" s="6">
-        <v>220954</v>
+        <v>330368</v>
       </c>
       <c r="Y137" s="6">
-        <v>221559</v>
+        <v>332609</v>
       </c>
       <c r="Z137" s="4"/>
     </row>
@@ -8907,76 +8926,76 @@
         <v>26</v>
       </c>
       <c r="B139" s="6">
-        <v>306169</v>
+        <v>561366</v>
       </c>
       <c r="C139" s="6">
-        <v>306152</v>
+        <v>557481</v>
       </c>
       <c r="D139" s="6">
-        <v>305729</v>
+        <v>554411</v>
       </c>
       <c r="E139" s="6">
-        <v>305216</v>
+        <v>549489</v>
       </c>
       <c r="F139" s="6">
-        <v>305493</v>
+        <v>545198</v>
       </c>
       <c r="G139" s="6">
-        <v>304957</v>
+        <v>541414</v>
       </c>
       <c r="H139" s="6">
-        <v>304066</v>
+        <v>537973</v>
       </c>
       <c r="I139" s="6">
-        <v>302889</v>
+        <v>533824</v>
       </c>
       <c r="J139" s="6">
-        <v>302357</v>
+        <v>531140</v>
       </c>
       <c r="K139" s="6">
-        <v>303783</v>
+        <v>531307</v>
       </c>
       <c r="L139" s="6">
-        <v>305306</v>
+        <v>531874</v>
       </c>
       <c r="M139" s="6">
-        <v>307323</v>
+        <v>532739</v>
       </c>
       <c r="N139" s="6">
-        <v>308132</v>
+        <v>532286</v>
       </c>
       <c r="O139" s="6">
-        <v>309347</v>
+        <v>532135</v>
       </c>
       <c r="P139" s="6">
-        <v>310460</v>
+        <v>533025</v>
       </c>
       <c r="Q139" s="6">
-        <v>311761</v>
+        <v>534079</v>
       </c>
       <c r="R139" s="6">
-        <v>313777</v>
+        <v>535796</v>
       </c>
       <c r="S139" s="6">
-        <v>315637</v>
+        <v>536781</v>
       </c>
       <c r="T139" s="6">
-        <v>318550</v>
+        <v>537668</v>
       </c>
       <c r="U139" s="6">
-        <v>321722</v>
+        <v>537513</v>
       </c>
       <c r="V139" s="6">
-        <v>324423</v>
+        <v>536167</v>
       </c>
       <c r="W139" s="6">
-        <v>327383</v>
+        <v>534262</v>
       </c>
       <c r="X139" s="6">
-        <v>330368</v>
+        <v>532036</v>
       </c>
       <c r="Y139" s="6">
-        <v>332609</v>
+        <v>528338</v>
       </c>
       <c r="Z139" s="4"/>
     </row>
@@ -9015,76 +9034,76 @@
         <v>26</v>
       </c>
       <c r="B141" s="6">
-        <v>561366</v>
+        <v>2662738</v>
       </c>
       <c r="C141" s="6">
-        <v>557481</v>
+        <v>2651628</v>
       </c>
       <c r="D141" s="6">
-        <v>554411</v>
+        <v>2641079</v>
       </c>
       <c r="E141" s="6">
-        <v>549489</v>
+        <v>2621050</v>
       </c>
       <c r="F141" s="6">
-        <v>545198</v>
+        <v>2602595</v>
       </c>
       <c r="G141" s="6">
-        <v>541414</v>
+        <v>2571987</v>
       </c>
       <c r="H141" s="6">
-        <v>537973</v>
+        <v>2539430</v>
       </c>
       <c r="I141" s="6">
-        <v>533824</v>
+        <v>2503510</v>
       </c>
       <c r="J141" s="6">
-        <v>531140</v>
+        <v>2473024</v>
       </c>
       <c r="K141" s="6">
-        <v>531307</v>
+        <v>2453455</v>
       </c>
       <c r="L141" s="6">
-        <v>531874</v>
+        <v>2438910</v>
       </c>
       <c r="M141" s="6">
-        <v>532739</v>
+        <v>2430765</v>
       </c>
       <c r="N141" s="6">
-        <v>532286</v>
+        <v>2417358</v>
       </c>
       <c r="O141" s="6">
-        <v>532135</v>
+        <v>2407230</v>
       </c>
       <c r="P141" s="6">
-        <v>533025</v>
+        <v>2398751</v>
       </c>
       <c r="Q141" s="6">
-        <v>534079</v>
+        <v>2390638</v>
       </c>
       <c r="R141" s="6">
-        <v>535796</v>
+        <v>2384812</v>
       </c>
       <c r="S141" s="6">
-        <v>536781</v>
+        <v>2376774</v>
       </c>
       <c r="T141" s="6">
-        <v>537668</v>
+        <v>2365680</v>
       </c>
       <c r="U141" s="6">
-        <v>537513</v>
+        <v>2350080</v>
       </c>
       <c r="V141" s="6">
-        <v>536167</v>
+        <v>2332813</v>
       </c>
       <c r="W141" s="6">
-        <v>534262</v>
+        <v>2317153</v>
       </c>
       <c r="X141" s="6">
-        <v>532036</v>
+        <v>2296353</v>
       </c>
       <c r="Y141" s="6">
-        <v>528338</v>
+        <v>2268179</v>
       </c>
       <c r="Z141" s="4"/>
     </row>
@@ -9123,80 +9142,80 @@
         <v>26</v>
       </c>
       <c r="B143" s="6">
-        <v>2662738</v>
+        <v>3048716</v>
       </c>
       <c r="C143" s="6">
-        <v>2651628</v>
+        <v>3022092</v>
       </c>
       <c r="D143" s="6">
-        <v>2641079</v>
+        <v>3000891</v>
       </c>
       <c r="E143" s="6">
-        <v>2621050</v>
+        <v>2981746</v>
       </c>
       <c r="F143" s="6">
-        <v>2602595</v>
+        <v>2961871</v>
       </c>
       <c r="G143" s="6">
-        <v>2571987</v>
+        <v>2931905</v>
       </c>
       <c r="H143" s="6">
-        <v>2539430</v>
+        <v>2901930</v>
       </c>
       <c r="I143" s="6">
-        <v>2503510</v>
+        <v>2869315</v>
       </c>
       <c r="J143" s="6">
-        <v>2473024</v>
+        <v>2845425</v>
       </c>
       <c r="K143" s="6">
-        <v>2453455</v>
+        <v>2837013</v>
       </c>
       <c r="L143" s="6">
-        <v>2438910</v>
+        <v>2832591</v>
       </c>
       <c r="M143" s="6">
-        <v>2430765</v>
+        <v>2832854</v>
       </c>
       <c r="N143" s="6">
-        <v>2417358</v>
+        <v>2829105</v>
       </c>
       <c r="O143" s="6">
-        <v>2407230</v>
+        <v>2838396</v>
       </c>
       <c r="P143" s="6">
-        <v>2398751</v>
+        <v>2846475</v>
       </c>
       <c r="Q143" s="6">
-        <v>2390638</v>
+        <v>2852810</v>
       </c>
       <c r="R143" s="6">
-        <v>2384812</v>
+        <v>2858773</v>
       </c>
       <c r="S143" s="6">
-        <v>2376774</v>
+        <v>2866490</v>
       </c>
       <c r="T143" s="6">
-        <v>2365680</v>
+        <v>2875301</v>
       </c>
       <c r="U143" s="6">
-        <v>2350080</v>
+        <v>2876497</v>
       </c>
       <c r="V143" s="6">
-        <v>2332813</v>
+        <v>2874026</v>
       </c>
       <c r="W143" s="6">
-        <v>2317153</v>
+        <v>2866255</v>
       </c>
       <c r="X143" s="6">
-        <v>2296353</v>
+        <v>2855899</v>
       </c>
       <c r="Y143" s="6">
-        <v>2268179</v>
+        <v>2849169</v>
       </c>
       <c r="Z143" s="4"/>
     </row>
-    <row r="144" ht="26.5" customHeight="1">
+    <row r="144" ht="14.5" customHeight="1">
       <c r="A144" t="s" s="2">
         <v>97</v>
       </c>
@@ -9231,37 +9250,77 @@
         <v>26</v>
       </c>
       <c r="B145" s="6">
-        <v>71325</v>
+        <v>2667886</v>
       </c>
       <c r="C145" s="6">
-        <v>71307</v>
+        <v>2644022</v>
       </c>
       <c r="D145" s="6">
-        <v>71162</v>
+        <v>2623183</v>
       </c>
       <c r="E145" s="6">
-        <v>71777</v>
-      </c>
-      <c r="F145" s="5"/>
-      <c r="G145" s="5"/>
-      <c r="H145" s="5"/>
-      <c r="I145" s="5"/>
-      <c r="J145" s="5"/>
-      <c r="K145" s="5"/>
-      <c r="L145" s="5"/>
-      <c r="M145" s="5"/>
-      <c r="N145" s="5"/>
-      <c r="O145" s="5"/>
-      <c r="P145" s="5"/>
-      <c r="Q145" s="5"/>
-      <c r="R145" s="5"/>
-      <c r="S145" s="5"/>
-      <c r="T145" s="5"/>
-      <c r="U145" s="5"/>
-      <c r="V145" s="5"/>
-      <c r="W145" s="5"/>
-      <c r="X145" s="5"/>
-      <c r="Y145" s="5"/>
+        <v>2599675</v>
+      </c>
+      <c r="F145" s="6">
+        <v>2577702</v>
+      </c>
+      <c r="G145" s="6">
+        <v>2552298</v>
+      </c>
+      <c r="H145" s="6">
+        <v>2524080</v>
+      </c>
+      <c r="I145" s="6">
+        <v>2492143</v>
+      </c>
+      <c r="J145" s="6">
+        <v>2467383</v>
+      </c>
+      <c r="K145" s="6">
+        <v>2455410</v>
+      </c>
+      <c r="L145" s="6">
+        <v>2448287</v>
+      </c>
+      <c r="M145" s="6">
+        <v>2440391</v>
+      </c>
+      <c r="N145" s="6">
+        <v>2427954</v>
+      </c>
+      <c r="O145" s="6">
+        <v>2424355</v>
+      </c>
+      <c r="P145" s="6">
+        <v>2422026</v>
+      </c>
+      <c r="Q145" s="6">
+        <v>2418348</v>
+      </c>
+      <c r="R145" s="6">
+        <v>2414913</v>
+      </c>
+      <c r="S145" s="6">
+        <v>2412800</v>
+      </c>
+      <c r="T145" s="6">
+        <v>2408901</v>
+      </c>
+      <c r="U145" s="6">
+        <v>2404195</v>
+      </c>
+      <c r="V145" s="6">
+        <v>2397763</v>
+      </c>
+      <c r="W145" s="6">
+        <v>2391193</v>
+      </c>
+      <c r="X145" s="6">
+        <v>2375021</v>
+      </c>
+      <c r="Y145" s="6">
+        <v>2357134</v>
+      </c>
       <c r="Z145" s="4"/>
     </row>
     <row r="146" ht="14.5" customHeight="1">
@@ -9299,80 +9358,80 @@
         <v>26</v>
       </c>
       <c r="B147" s="6">
-        <v>3048716</v>
+        <v>2985392</v>
       </c>
       <c r="C147" s="6">
-        <v>3022092</v>
+        <v>2963439</v>
       </c>
       <c r="D147" s="6">
-        <v>3000891</v>
+        <v>2942264</v>
       </c>
       <c r="E147" s="6">
-        <v>2981746</v>
+        <v>2917769</v>
       </c>
       <c r="F147" s="6">
-        <v>2961871</v>
+        <v>2893448</v>
       </c>
       <c r="G147" s="6">
-        <v>2931905</v>
+        <v>2862105</v>
       </c>
       <c r="H147" s="6">
-        <v>2901930</v>
+        <v>2832963</v>
       </c>
       <c r="I147" s="6">
-        <v>2869315</v>
+        <v>2805941</v>
       </c>
       <c r="J147" s="6">
-        <v>2845425</v>
+        <v>2785999</v>
       </c>
       <c r="K147" s="6">
-        <v>2837013</v>
+        <v>2780231</v>
       </c>
       <c r="L147" s="6">
-        <v>2832591</v>
+        <v>2776358</v>
       </c>
       <c r="M147" s="6">
-        <v>2832854</v>
+        <v>2772964</v>
       </c>
       <c r="N147" s="6">
-        <v>2829105</v>
+        <v>2761255</v>
       </c>
       <c r="O147" s="6">
-        <v>2838396</v>
+        <v>2750829</v>
       </c>
       <c r="P147" s="6">
-        <v>2846475</v>
+        <v>2742450</v>
       </c>
       <c r="Q147" s="6">
-        <v>2852810</v>
+        <v>2734075</v>
       </c>
       <c r="R147" s="6">
-        <v>2858773</v>
+        <v>2724990</v>
       </c>
       <c r="S147" s="6">
-        <v>2866490</v>
+        <v>2717627</v>
       </c>
       <c r="T147" s="6">
-        <v>2875301</v>
+        <v>2708844</v>
       </c>
       <c r="U147" s="6">
-        <v>2876497</v>
+        <v>2694877</v>
       </c>
       <c r="V147" s="6">
-        <v>2874026</v>
+        <v>2674256</v>
       </c>
       <c r="W147" s="6">
-        <v>2866255</v>
+        <v>2657854</v>
       </c>
       <c r="X147" s="6">
-        <v>2855899</v>
+        <v>2633446</v>
       </c>
       <c r="Y147" s="6">
-        <v>2849169</v>
+        <v>2604272</v>
       </c>
       <c r="Z147" s="4"/>
     </row>
-    <row r="148" ht="38.5" customHeight="1">
+    <row r="148" ht="14.5" customHeight="1">
       <c r="A148" t="s" s="2">
         <v>99</v>
       </c>
@@ -9407,40 +9466,80 @@
         <v>26</v>
       </c>
       <c r="B149" s="6">
-        <v>39026</v>
+        <v>2734031</v>
       </c>
       <c r="C149" s="6">
-        <v>38263</v>
+        <v>2725499</v>
       </c>
       <c r="D149" s="6">
-        <v>38250</v>
+        <v>2715128</v>
       </c>
       <c r="E149" s="6">
-        <v>39160</v>
-      </c>
-      <c r="F149" s="5"/>
-      <c r="G149" s="5"/>
-      <c r="H149" s="5"/>
-      <c r="I149" s="5"/>
-      <c r="J149" s="5"/>
-      <c r="K149" s="5"/>
-      <c r="L149" s="5"/>
-      <c r="M149" s="5"/>
-      <c r="N149" s="5"/>
-      <c r="O149" s="5"/>
-      <c r="P149" s="5"/>
-      <c r="Q149" s="5"/>
-      <c r="R149" s="5"/>
-      <c r="S149" s="5"/>
-      <c r="T149" s="5"/>
-      <c r="U149" s="5"/>
-      <c r="V149" s="5"/>
-      <c r="W149" s="5"/>
-      <c r="X149" s="5"/>
-      <c r="Y149" s="5"/>
+        <v>2703012</v>
+      </c>
+      <c r="F149" s="6">
+        <v>2688423</v>
+      </c>
+      <c r="G149" s="6">
+        <v>2674155</v>
+      </c>
+      <c r="H149" s="6">
+        <v>2665984</v>
+      </c>
+      <c r="I149" s="6">
+        <v>2654853</v>
+      </c>
+      <c r="J149" s="6">
+        <v>2647195</v>
+      </c>
+      <c r="K149" s="6">
+        <v>2642727</v>
+      </c>
+      <c r="L149" s="6">
+        <v>2648923</v>
+      </c>
+      <c r="M149" s="6">
+        <v>2661594</v>
+      </c>
+      <c r="N149" s="6">
+        <v>2666465</v>
+      </c>
+      <c r="O149" s="6">
+        <v>2686863</v>
+      </c>
+      <c r="P149" s="6">
+        <v>2709461</v>
+      </c>
+      <c r="Q149" s="6">
+        <v>2731176</v>
+      </c>
+      <c r="R149" s="6">
+        <v>2746822</v>
+      </c>
+      <c r="S149" s="6">
+        <v>2762237</v>
+      </c>
+      <c r="T149" s="6">
+        <v>2779555</v>
+      </c>
+      <c r="U149" s="6">
+        <v>2788849</v>
+      </c>
+      <c r="V149" s="6">
+        <v>2793384</v>
+      </c>
+      <c r="W149" s="6">
+        <v>2798170</v>
+      </c>
+      <c r="X149" s="6">
+        <v>2785836</v>
+      </c>
+      <c r="Y149" s="6">
+        <v>2780292</v>
+      </c>
       <c r="Z149" s="4"/>
     </row>
-    <row r="150" ht="26.5" customHeight="1">
+    <row r="150" ht="14.5" customHeight="1">
       <c r="A150" t="s" s="2">
         <v>100</v>
       </c>
@@ -9475,37 +9574,77 @@
         <v>26</v>
       </c>
       <c r="B151" s="6">
-        <v>19014</v>
+        <v>2153911</v>
       </c>
       <c r="C151" s="6">
-        <v>18469</v>
+        <v>2136058</v>
       </c>
       <c r="D151" s="6">
-        <v>18012</v>
+        <v>2117291</v>
       </c>
       <c r="E151" s="6">
-        <v>17751</v>
-      </c>
-      <c r="F151" s="5"/>
-      <c r="G151" s="5"/>
-      <c r="H151" s="5"/>
-      <c r="I151" s="5"/>
-      <c r="J151" s="5"/>
-      <c r="K151" s="5"/>
-      <c r="L151" s="5"/>
-      <c r="M151" s="5"/>
-      <c r="N151" s="5"/>
-      <c r="O151" s="5"/>
-      <c r="P151" s="5"/>
-      <c r="Q151" s="5"/>
-      <c r="R151" s="5"/>
-      <c r="S151" s="5"/>
-      <c r="T151" s="5"/>
-      <c r="U151" s="5"/>
-      <c r="V151" s="5"/>
-      <c r="W151" s="5"/>
-      <c r="X151" s="5"/>
-      <c r="Y151" s="5"/>
+        <v>2094735</v>
+      </c>
+      <c r="F151" s="6">
+        <v>2075422</v>
+      </c>
+      <c r="G151" s="6">
+        <v>2052741</v>
+      </c>
+      <c r="H151" s="6">
+        <v>2034091</v>
+      </c>
+      <c r="I151" s="6">
+        <v>2016288</v>
+      </c>
+      <c r="J151" s="6">
+        <v>2003282</v>
+      </c>
+      <c r="K151" s="6">
+        <v>1993290</v>
+      </c>
+      <c r="L151" s="6">
+        <v>1987716</v>
+      </c>
+      <c r="M151" s="6">
+        <v>1983985</v>
+      </c>
+      <c r="N151" s="6">
+        <v>1976560</v>
+      </c>
+      <c r="O151" s="6">
+        <v>1974820</v>
+      </c>
+      <c r="P151" s="6">
+        <v>1973985</v>
+      </c>
+      <c r="Q151" s="6">
+        <v>1973876</v>
+      </c>
+      <c r="R151" s="6">
+        <v>1978183</v>
+      </c>
+      <c r="S151" s="6">
+        <v>1978466</v>
+      </c>
+      <c r="T151" s="6">
+        <v>1972682</v>
+      </c>
+      <c r="U151" s="6">
+        <v>1960081</v>
+      </c>
+      <c r="V151" s="6">
+        <v>1944195</v>
+      </c>
+      <c r="W151" s="6">
+        <v>1926665</v>
+      </c>
+      <c r="X151" s="6">
+        <v>1903675</v>
+      </c>
+      <c r="Y151" s="6">
+        <v>1879548</v>
+      </c>
       <c r="Z151" s="4"/>
     </row>
     <row r="152" ht="14.5" customHeight="1">
@@ -9543,76 +9682,76 @@
         <v>26</v>
       </c>
       <c r="B153" s="6">
-        <v>2667886</v>
+        <v>1062469</v>
       </c>
       <c r="C153" s="6">
-        <v>2644022</v>
+        <v>1057846</v>
       </c>
       <c r="D153" s="6">
-        <v>2623183</v>
+        <v>1054272</v>
       </c>
       <c r="E153" s="6">
-        <v>2599675</v>
+        <v>1049770</v>
       </c>
       <c r="F153" s="6">
-        <v>2577702</v>
+        <v>1045539</v>
       </c>
       <c r="G153" s="6">
-        <v>2552298</v>
+        <v>1037952</v>
       </c>
       <c r="H153" s="6">
-        <v>2524080</v>
+        <v>1029944</v>
       </c>
       <c r="I153" s="6">
-        <v>2492143</v>
+        <v>1024294</v>
       </c>
       <c r="J153" s="6">
-        <v>2467383</v>
+        <v>1023063</v>
       </c>
       <c r="K153" s="6">
-        <v>2455410</v>
+        <v>1026307</v>
       </c>
       <c r="L153" s="6">
-        <v>2448287</v>
+        <v>1031522</v>
       </c>
       <c r="M153" s="6">
-        <v>2440391</v>
+        <v>1040245</v>
       </c>
       <c r="N153" s="6">
-        <v>2427954</v>
+        <v>1048538</v>
       </c>
       <c r="O153" s="6">
-        <v>2424355</v>
+        <v>1057748</v>
       </c>
       <c r="P153" s="6">
-        <v>2422026</v>
+        <v>1064245</v>
       </c>
       <c r="Q153" s="6">
-        <v>2418348</v>
+        <v>1070128</v>
       </c>
       <c r="R153" s="6">
-        <v>2414913</v>
+        <v>1074453</v>
       </c>
       <c r="S153" s="6">
-        <v>2412800</v>
+        <v>1076762</v>
       </c>
       <c r="T153" s="6">
-        <v>2408901</v>
+        <v>1078891</v>
       </c>
       <c r="U153" s="6">
-        <v>2404195</v>
+        <v>1078280</v>
       </c>
       <c r="V153" s="6">
-        <v>2397763</v>
+        <v>1077442</v>
       </c>
       <c r="W153" s="6">
-        <v>2391193</v>
+        <v>1079271</v>
       </c>
       <c r="X153" s="6">
-        <v>2375021</v>
+        <v>1070339</v>
       </c>
       <c r="Y153" s="6">
-        <v>2357134</v>
+        <v>1068304</v>
       </c>
       <c r="Z153" s="4"/>
     </row>
@@ -9651,76 +9790,76 @@
         <v>26</v>
       </c>
       <c r="B155" s="6">
-        <v>2985392</v>
+        <v>1013433</v>
       </c>
       <c r="C155" s="6">
-        <v>2963439</v>
+        <v>1004808</v>
       </c>
       <c r="D155" s="6">
-        <v>2942264</v>
+        <v>996912</v>
       </c>
       <c r="E155" s="6">
-        <v>2917769</v>
+        <v>987289</v>
       </c>
       <c r="F155" s="6">
-        <v>2893448</v>
+        <v>979605</v>
       </c>
       <c r="G155" s="6">
-        <v>2862105</v>
+        <v>974561</v>
       </c>
       <c r="H155" s="6">
-        <v>2832963</v>
+        <v>970994</v>
       </c>
       <c r="I155" s="6">
-        <v>2805941</v>
+        <v>966914</v>
       </c>
       <c r="J155" s="6">
-        <v>2785999</v>
+        <v>964581</v>
       </c>
       <c r="K155" s="6">
-        <v>2780231</v>
+        <v>965156</v>
       </c>
       <c r="L155" s="6">
-        <v>2776358</v>
+        <v>966595</v>
       </c>
       <c r="M155" s="6">
-        <v>2772964</v>
+        <v>969736</v>
       </c>
       <c r="N155" s="6">
-        <v>2761255</v>
+        <v>971538</v>
       </c>
       <c r="O155" s="6">
-        <v>2750829</v>
+        <v>971391</v>
       </c>
       <c r="P155" s="6">
-        <v>2742450</v>
+        <v>971810</v>
       </c>
       <c r="Q155" s="6">
-        <v>2734075</v>
+        <v>973860</v>
       </c>
       <c r="R155" s="6">
-        <v>2724990</v>
+        <v>978495</v>
       </c>
       <c r="S155" s="6">
-        <v>2717627</v>
+        <v>982284</v>
       </c>
       <c r="T155" s="6">
-        <v>2708844</v>
+        <v>984134</v>
       </c>
       <c r="U155" s="6">
-        <v>2694877</v>
+        <v>984511</v>
       </c>
       <c r="V155" s="6">
-        <v>2674256</v>
+        <v>983273</v>
       </c>
       <c r="W155" s="6">
-        <v>2657854</v>
+        <v>985937</v>
       </c>
       <c r="X155" s="6">
-        <v>2633446</v>
+        <v>985431</v>
       </c>
       <c r="Y155" s="6">
-        <v>2604272</v>
+        <v>982629</v>
       </c>
       <c r="Z155" s="4"/>
     </row>
@@ -9759,37 +9898,77 @@
         <v>26</v>
       </c>
       <c r="B157" s="6">
-        <v>134461</v>
+        <v>1207030</v>
       </c>
       <c r="C157" s="6">
-        <v>134694</v>
+        <v>1192819</v>
       </c>
       <c r="D157" s="6">
-        <v>134735</v>
+        <v>1178824</v>
       </c>
       <c r="E157" s="6">
-        <v>135210</v>
-      </c>
-      <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
-      <c r="H157" s="5"/>
-      <c r="I157" s="5"/>
-      <c r="J157" s="5"/>
-      <c r="K157" s="5"/>
-      <c r="L157" s="5"/>
-      <c r="M157" s="5"/>
-      <c r="N157" s="5"/>
-      <c r="O157" s="5"/>
-      <c r="P157" s="5"/>
-      <c r="Q157" s="5"/>
-      <c r="R157" s="5"/>
-      <c r="S157" s="5"/>
-      <c r="T157" s="5"/>
-      <c r="U157" s="5"/>
-      <c r="V157" s="5"/>
-      <c r="W157" s="5"/>
-      <c r="X157" s="5"/>
-      <c r="Y157" s="5"/>
+        <v>1165435</v>
+      </c>
+      <c r="F157" s="6">
+        <v>1152596</v>
+      </c>
+      <c r="G157" s="6">
+        <v>1142687</v>
+      </c>
+      <c r="H157" s="6">
+        <v>1132780</v>
+      </c>
+      <c r="I157" s="6">
+        <v>1123327</v>
+      </c>
+      <c r="J157" s="6">
+        <v>1115143</v>
+      </c>
+      <c r="K157" s="6">
+        <v>1111439</v>
+      </c>
+      <c r="L157" s="6">
+        <v>1109196</v>
+      </c>
+      <c r="M157" s="6">
+        <v>1108973</v>
+      </c>
+      <c r="N157" s="6">
+        <v>1106155</v>
+      </c>
+      <c r="O157" s="6">
+        <v>1099396</v>
+      </c>
+      <c r="P157" s="6">
+        <v>1095169</v>
+      </c>
+      <c r="Q157" s="6">
+        <v>1090344</v>
+      </c>
+      <c r="R157" s="6">
+        <v>1087452</v>
+      </c>
+      <c r="S157" s="6">
+        <v>1083012</v>
+      </c>
+      <c r="T157" s="6">
+        <v>1078983</v>
+      </c>
+      <c r="U157" s="6">
+        <v>1072806</v>
+      </c>
+      <c r="V157" s="6">
+        <v>1065785</v>
+      </c>
+      <c r="W157" s="6">
+        <v>1059700</v>
+      </c>
+      <c r="X157" s="6">
+        <v>1053485</v>
+      </c>
+      <c r="Y157" s="6">
+        <v>1043467</v>
+      </c>
       <c r="Z157" s="4"/>
     </row>
     <row r="158" ht="14.5" customHeight="1">
@@ -9827,76 +10006,76 @@
         <v>26</v>
       </c>
       <c r="B159" s="6">
-        <v>2734031</v>
+        <v>977117</v>
       </c>
       <c r="C159" s="6">
-        <v>2725499</v>
+        <v>962507</v>
       </c>
       <c r="D159" s="6">
-        <v>2715128</v>
+        <v>957478</v>
       </c>
       <c r="E159" s="6">
-        <v>2703012</v>
+        <v>951478</v>
       </c>
       <c r="F159" s="6">
-        <v>2688423</v>
+        <v>948636</v>
       </c>
       <c r="G159" s="6">
-        <v>2674155</v>
+        <v>949969</v>
       </c>
       <c r="H159" s="6">
-        <v>2665984</v>
+        <v>953170</v>
       </c>
       <c r="I159" s="6">
-        <v>2654853</v>
+        <v>954394</v>
       </c>
       <c r="J159" s="6">
-        <v>2647195</v>
+        <v>956099</v>
       </c>
       <c r="K159" s="6">
-        <v>2642727</v>
+        <v>958929</v>
       </c>
       <c r="L159" s="6">
-        <v>2648923</v>
+        <v>958056</v>
       </c>
       <c r="M159" s="6">
-        <v>2661594</v>
+        <v>958338</v>
       </c>
       <c r="N159" s="6">
-        <v>2666465</v>
+        <v>958258</v>
       </c>
       <c r="O159" s="6">
-        <v>2686863</v>
+        <v>955859</v>
       </c>
       <c r="P159" s="6">
-        <v>2709461</v>
+        <v>955580</v>
       </c>
       <c r="Q159" s="6">
-        <v>2731176</v>
+        <v>954803</v>
       </c>
       <c r="R159" s="6">
-        <v>2746822</v>
+        <v>956896</v>
       </c>
       <c r="S159" s="6">
-        <v>2762237</v>
+        <v>959689</v>
       </c>
       <c r="T159" s="6">
-        <v>2779555</v>
+        <v>962835</v>
       </c>
       <c r="U159" s="6">
-        <v>2788849</v>
+        <v>964330</v>
       </c>
       <c r="V159" s="6">
-        <v>2793384</v>
+        <v>967009</v>
       </c>
       <c r="W159" s="6">
-        <v>2798170</v>
+        <v>971996</v>
       </c>
       <c r="X159" s="6">
-        <v>2785836</v>
+        <v>981971</v>
       </c>
       <c r="Y159" s="6">
-        <v>2780292</v>
+        <v>992115</v>
       </c>
       <c r="Z159" s="4"/>
     </row>
@@ -9935,76 +10114,76 @@
         <v>26</v>
       </c>
       <c r="B161" s="6">
-        <v>2153911</v>
+        <v>380481</v>
       </c>
       <c r="C161" s="6">
-        <v>2136058</v>
+        <v>372308</v>
       </c>
       <c r="D161" s="6">
-        <v>2117291</v>
+        <v>366400</v>
       </c>
       <c r="E161" s="6">
-        <v>2094735</v>
+        <v>361646</v>
       </c>
       <c r="F161" s="6">
-        <v>2075422</v>
+        <v>357917</v>
       </c>
       <c r="G161" s="6">
-        <v>2052741</v>
+        <v>350510</v>
       </c>
       <c r="H161" s="6">
-        <v>2034091</v>
+        <v>343908</v>
       </c>
       <c r="I161" s="6">
-        <v>2016288</v>
+        <v>336594</v>
       </c>
       <c r="J161" s="6">
-        <v>2003282</v>
+        <v>330810</v>
       </c>
       <c r="K161" s="6">
-        <v>1993290</v>
+        <v>327949</v>
       </c>
       <c r="L161" s="6">
-        <v>1987716</v>
+        <v>325179</v>
       </c>
       <c r="M161" s="6">
-        <v>1983985</v>
+        <v>323165</v>
       </c>
       <c r="N161" s="6">
-        <v>1976560</v>
+        <v>321659</v>
       </c>
       <c r="O161" s="6">
-        <v>1974820</v>
+        <v>320156</v>
       </c>
       <c r="P161" s="6">
-        <v>1973985</v>
+        <v>320549</v>
       </c>
       <c r="Q161" s="6">
-        <v>1973876</v>
+        <v>319864</v>
       </c>
       <c r="R161" s="6">
-        <v>1978183</v>
+        <v>317269</v>
       </c>
       <c r="S161" s="6">
-        <v>1978466</v>
+        <v>316116</v>
       </c>
       <c r="T161" s="6">
-        <v>1972682</v>
+        <v>314729</v>
       </c>
       <c r="U161" s="6">
-        <v>1960081</v>
+        <v>315557</v>
       </c>
       <c r="V161" s="6">
-        <v>1944195</v>
+        <v>314723</v>
       </c>
       <c r="W161" s="6">
-        <v>1926665</v>
+        <v>313016</v>
       </c>
       <c r="X161" s="6">
-        <v>1903675</v>
+        <v>311667</v>
       </c>
       <c r="Y161" s="6">
-        <v>1879548</v>
+        <v>312704</v>
       </c>
       <c r="Z161" s="4"/>
     </row>
@@ -10043,76 +10222,76 @@
         <v>26</v>
       </c>
       <c r="B163" s="6">
-        <v>1062469</v>
+        <v>2167274</v>
       </c>
       <c r="C163" s="6">
-        <v>1057846</v>
+        <v>2141025</v>
       </c>
       <c r="D163" s="6">
-        <v>1054272</v>
+        <v>2120467</v>
       </c>
       <c r="E163" s="6">
-        <v>1049770</v>
+        <v>2085743</v>
       </c>
       <c r="F163" s="6">
-        <v>1045539</v>
+        <v>2067342</v>
       </c>
       <c r="G163" s="6">
-        <v>1037952</v>
+        <v>2048582</v>
       </c>
       <c r="H163" s="6">
-        <v>1029944</v>
+        <v>2028377</v>
       </c>
       <c r="I163" s="6">
-        <v>1024294</v>
+        <v>2006536</v>
       </c>
       <c r="J163" s="6">
-        <v>1023063</v>
+        <v>1988580</v>
       </c>
       <c r="K163" s="6">
-        <v>1026307</v>
+        <v>1977392</v>
       </c>
       <c r="L163" s="6">
-        <v>1031522</v>
+        <v>1969602</v>
       </c>
       <c r="M163" s="6">
-        <v>1040245</v>
+        <v>1965178</v>
       </c>
       <c r="N163" s="6">
-        <v>1048538</v>
+        <v>1953545</v>
       </c>
       <c r="O163" s="6">
-        <v>1057748</v>
+        <v>1950483</v>
       </c>
       <c r="P163" s="6">
-        <v>1064245</v>
+        <v>1947263</v>
       </c>
       <c r="Q163" s="6">
-        <v>1070128</v>
+        <v>1938516</v>
       </c>
       <c r="R163" s="6">
-        <v>1074453</v>
+        <v>1933308</v>
       </c>
       <c r="S163" s="6">
-        <v>1076762</v>
+        <v>1929008</v>
       </c>
       <c r="T163" s="6">
-        <v>1078891</v>
+        <v>1923116</v>
       </c>
       <c r="U163" s="6">
-        <v>1078280</v>
+        <v>1913037</v>
       </c>
       <c r="V163" s="6">
-        <v>1077442</v>
+        <v>1902718</v>
       </c>
       <c r="W163" s="6">
-        <v>1079271</v>
+        <v>1895868</v>
       </c>
       <c r="X163" s="6">
-        <v>1070339</v>
+        <v>1877844</v>
       </c>
       <c r="Y163" s="6">
-        <v>1068304</v>
+        <v>1863011</v>
       </c>
       <c r="Z163" s="4"/>
     </row>
@@ -10151,76 +10330,76 @@
         <v>26</v>
       </c>
       <c r="B165" s="6">
-        <v>1013433</v>
+        <v>1493881</v>
       </c>
       <c r="C165" s="6">
-        <v>1004808</v>
+        <v>1473876</v>
       </c>
       <c r="D165" s="6">
-        <v>996912</v>
+        <v>1459908</v>
       </c>
       <c r="E165" s="6">
-        <v>987289</v>
+        <v>1446177</v>
       </c>
       <c r="F165" s="6">
-        <v>979605</v>
+        <v>1434242</v>
       </c>
       <c r="G165" s="6">
-        <v>974561</v>
+        <v>1416224</v>
       </c>
       <c r="H165" s="6">
-        <v>970994</v>
+        <v>1396800</v>
       </c>
       <c r="I165" s="6">
-        <v>966914</v>
+        <v>1376260</v>
       </c>
       <c r="J165" s="6">
-        <v>964581</v>
+        <v>1359894</v>
       </c>
       <c r="K165" s="6">
-        <v>965156</v>
+        <v>1354848</v>
       </c>
       <c r="L165" s="6">
-        <v>966595</v>
+        <v>1351123</v>
       </c>
       <c r="M165" s="6">
-        <v>969736</v>
+        <v>1349230</v>
       </c>
       <c r="N165" s="6">
-        <v>971538</v>
+        <v>1342887</v>
       </c>
       <c r="O165" s="6">
-        <v>971391</v>
+        <v>1342475</v>
       </c>
       <c r="P165" s="6">
-        <v>971810</v>
+        <v>1342083</v>
       </c>
       <c r="Q165" s="6">
-        <v>973860</v>
+        <v>1339912</v>
       </c>
       <c r="R165" s="6">
-        <v>978495</v>
+        <v>1338305</v>
       </c>
       <c r="S165" s="6">
-        <v>982284</v>
+        <v>1334552</v>
       </c>
       <c r="T165" s="6">
-        <v>984134</v>
+        <v>1333294</v>
       </c>
       <c r="U165" s="6">
-        <v>984511</v>
+        <v>1328302</v>
       </c>
       <c r="V165" s="6">
-        <v>983273</v>
+        <v>1321473</v>
       </c>
       <c r="W165" s="6">
-        <v>985937</v>
+        <v>1315643</v>
       </c>
       <c r="X165" s="6">
-        <v>985431</v>
+        <v>1301127</v>
       </c>
       <c r="Y165" s="6">
-        <v>982629</v>
+        <v>1298978</v>
       </c>
       <c r="Z165" s="4"/>
     </row>
@@ -10259,76 +10438,76 @@
         <v>26</v>
       </c>
       <c r="B167" s="6">
-        <v>1207030</v>
+        <v>949526</v>
       </c>
       <c r="C167" s="6">
-        <v>1192819</v>
+        <v>935607</v>
       </c>
       <c r="D167" s="6">
-        <v>1178824</v>
+        <v>923055</v>
       </c>
       <c r="E167" s="6">
-        <v>1165435</v>
+        <v>911381</v>
       </c>
       <c r="F167" s="6">
-        <v>1152596</v>
+        <v>901044</v>
       </c>
       <c r="G167" s="6">
-        <v>1142687</v>
+        <v>887781</v>
       </c>
       <c r="H167" s="6">
-        <v>1132780</v>
+        <v>874018</v>
       </c>
       <c r="I167" s="6">
-        <v>1123327</v>
+        <v>861056</v>
       </c>
       <c r="J167" s="6">
-        <v>1115143</v>
+        <v>850502</v>
       </c>
       <c r="K167" s="6">
-        <v>1111439</v>
+        <v>844290</v>
       </c>
       <c r="L167" s="6">
-        <v>1109196</v>
+        <v>838869</v>
       </c>
       <c r="M167" s="6">
-        <v>1108973</v>
+        <v>834905</v>
       </c>
       <c r="N167" s="6">
-        <v>1106155</v>
+        <v>828660</v>
       </c>
       <c r="O167" s="6">
-        <v>1099396</v>
+        <v>821573</v>
       </c>
       <c r="P167" s="6">
-        <v>1095169</v>
+        <v>816910</v>
       </c>
       <c r="Q167" s="6">
-        <v>1090344</v>
+        <v>811274</v>
       </c>
       <c r="R167" s="6">
-        <v>1087452</v>
+        <v>809873</v>
       </c>
       <c r="S167" s="6">
-        <v>1083012</v>
+        <v>805689</v>
       </c>
       <c r="T167" s="6">
-        <v>1078983</v>
+        <v>801752</v>
       </c>
       <c r="U167" s="6">
-        <v>1072806</v>
+        <v>798424</v>
       </c>
       <c r="V167" s="6">
-        <v>1065785</v>
+        <v>793194</v>
       </c>
       <c r="W167" s="6">
-        <v>1059700</v>
+        <v>790044</v>
       </c>
       <c r="X167" s="6">
-        <v>1053485</v>
+        <v>781846</v>
       </c>
       <c r="Y167" s="6">
-        <v>1043467</v>
+        <v>772525</v>
       </c>
       <c r="Z167" s="4"/>
     </row>
@@ -10367,76 +10546,76 @@
         <v>26</v>
       </c>
       <c r="B169" s="6">
-        <v>977117</v>
+        <v>211696</v>
       </c>
       <c r="C169" s="6">
-        <v>962507</v>
+        <v>201974</v>
       </c>
       <c r="D169" s="6">
-        <v>957478</v>
+        <v>193945</v>
       </c>
       <c r="E169" s="6">
-        <v>951478</v>
+        <v>187218</v>
       </c>
       <c r="F169" s="6">
-        <v>948636</v>
+        <v>181832</v>
       </c>
       <c r="G169" s="6">
-        <v>949969</v>
+        <v>178069</v>
       </c>
       <c r="H169" s="6">
-        <v>953170</v>
+        <v>173937</v>
       </c>
       <c r="I169" s="6">
-        <v>954394</v>
+        <v>170397</v>
       </c>
       <c r="J169" s="6">
-        <v>956099</v>
+        <v>166902</v>
       </c>
       <c r="K169" s="6">
-        <v>958929</v>
+        <v>163989</v>
       </c>
       <c r="L169" s="6">
-        <v>958056</v>
+        <v>160940</v>
       </c>
       <c r="M169" s="6">
-        <v>958338</v>
+        <v>159002</v>
       </c>
       <c r="N169" s="6">
-        <v>958258</v>
+        <v>156534</v>
       </c>
       <c r="O169" s="6">
-        <v>955859</v>
+        <v>154485</v>
       </c>
       <c r="P169" s="6">
-        <v>955580</v>
+        <v>152358</v>
       </c>
       <c r="Q169" s="6">
-        <v>954803</v>
+        <v>150312</v>
       </c>
       <c r="R169" s="6">
-        <v>956896</v>
+        <v>148071</v>
       </c>
       <c r="S169" s="6">
-        <v>959689</v>
+        <v>146345</v>
       </c>
       <c r="T169" s="6">
-        <v>962835</v>
+        <v>145570</v>
       </c>
       <c r="U169" s="6">
-        <v>964330</v>
+        <v>144091</v>
       </c>
       <c r="V169" s="6">
-        <v>967009</v>
+        <v>141234</v>
       </c>
       <c r="W169" s="6">
-        <v>971996</v>
+        <v>140149</v>
       </c>
       <c r="X169" s="6">
-        <v>981971</v>
+        <v>139034</v>
       </c>
       <c r="Y169" s="6">
-        <v>992115</v>
+        <v>137767</v>
       </c>
       <c r="Z169" s="4"/>
     </row>
@@ -10475,80 +10654,80 @@
         <v>26</v>
       </c>
       <c r="B171" s="6">
-        <v>380481</v>
+        <v>581305</v>
       </c>
       <c r="C171" s="6">
-        <v>372308</v>
+        <v>569234</v>
       </c>
       <c r="D171" s="6">
-        <v>366400</v>
+        <v>560049</v>
       </c>
       <c r="E171" s="6">
-        <v>361646</v>
+        <v>552155</v>
       </c>
       <c r="F171" s="6">
-        <v>357917</v>
+        <v>545008</v>
       </c>
       <c r="G171" s="6">
-        <v>350510</v>
+        <v>536783</v>
       </c>
       <c r="H171" s="6">
-        <v>343908</v>
+        <v>529813</v>
       </c>
       <c r="I171" s="6">
-        <v>336594</v>
+        <v>521121</v>
       </c>
       <c r="J171" s="6">
-        <v>330810</v>
+        <v>513452</v>
       </c>
       <c r="K171" s="6">
-        <v>327949</v>
+        <v>509364</v>
       </c>
       <c r="L171" s="6">
-        <v>325179</v>
+        <v>504896</v>
       </c>
       <c r="M171" s="6">
-        <v>323165</v>
+        <v>501279</v>
       </c>
       <c r="N171" s="6">
-        <v>321659</v>
+        <v>496739</v>
       </c>
       <c r="O171" s="6">
-        <v>320156</v>
+        <v>495402</v>
       </c>
       <c r="P171" s="6">
-        <v>320549</v>
+        <v>493302</v>
       </c>
       <c r="Q171" s="6">
-        <v>319864</v>
+        <v>491027</v>
       </c>
       <c r="R171" s="6">
-        <v>317269</v>
+        <v>488391</v>
       </c>
       <c r="S171" s="6">
-        <v>316116</v>
+        <v>487293</v>
       </c>
       <c r="T171" s="6">
-        <v>314729</v>
+        <v>487344</v>
       </c>
       <c r="U171" s="6">
-        <v>315557</v>
+        <v>490181</v>
       </c>
       <c r="V171" s="6">
-        <v>314723</v>
+        <v>489638</v>
       </c>
       <c r="W171" s="6">
-        <v>313016</v>
+        <v>488257</v>
       </c>
       <c r="X171" s="6">
-        <v>311667</v>
+        <v>485621</v>
       </c>
       <c r="Y171" s="6">
-        <v>312704</v>
+        <v>484177</v>
       </c>
       <c r="Z171" s="4"/>
     </row>
-    <row r="172" ht="26.5" customHeight="1">
+    <row r="172" ht="14.5" customHeight="1">
       <c r="A172" t="s" s="2">
         <v>111</v>
       </c>
@@ -10583,37 +10762,77 @@
         <v>26</v>
       </c>
       <c r="B173" s="6">
-        <v>27480</v>
+        <v>199172</v>
       </c>
       <c r="C173" s="6">
-        <v>26645</v>
+        <v>195135</v>
       </c>
       <c r="D173" s="6">
-        <v>25831</v>
+        <v>193198</v>
       </c>
       <c r="E173" s="6">
-        <v>25685</v>
-      </c>
-      <c r="F173" s="5"/>
-      <c r="G173" s="5"/>
-      <c r="H173" s="5"/>
-      <c r="I173" s="5"/>
-      <c r="J173" s="5"/>
-      <c r="K173" s="5"/>
-      <c r="L173" s="5"/>
-      <c r="M173" s="5"/>
-      <c r="N173" s="5"/>
-      <c r="O173" s="5"/>
-      <c r="P173" s="5"/>
-      <c r="Q173" s="5"/>
-      <c r="R173" s="5"/>
-      <c r="S173" s="5"/>
-      <c r="T173" s="5"/>
-      <c r="U173" s="5"/>
-      <c r="V173" s="5"/>
-      <c r="W173" s="5"/>
-      <c r="X173" s="5"/>
-      <c r="Y173" s="5"/>
+        <v>191899</v>
+      </c>
+      <c r="F173" s="6">
+        <v>190585</v>
+      </c>
+      <c r="G173" s="6">
+        <v>188412</v>
+      </c>
+      <c r="H173" s="6">
+        <v>185763</v>
+      </c>
+      <c r="I173" s="6">
+        <v>181653</v>
+      </c>
+      <c r="J173" s="6">
+        <v>179405</v>
+      </c>
+      <c r="K173" s="6">
+        <v>178711</v>
+      </c>
+      <c r="L173" s="6">
+        <v>178148</v>
+      </c>
+      <c r="M173" s="6">
+        <v>177500</v>
+      </c>
+      <c r="N173" s="6">
+        <v>176304</v>
+      </c>
+      <c r="O173" s="6">
+        <v>174412</v>
+      </c>
+      <c r="P173" s="6">
+        <v>172671</v>
+      </c>
+      <c r="Q173" s="6">
+        <v>170377</v>
+      </c>
+      <c r="R173" s="6">
+        <v>168368</v>
+      </c>
+      <c r="S173" s="6">
+        <v>166120</v>
+      </c>
+      <c r="T173" s="6">
+        <v>164217</v>
+      </c>
+      <c r="U173" s="6">
+        <v>162014</v>
+      </c>
+      <c r="V173" s="6">
+        <v>159913</v>
+      </c>
+      <c r="W173" s="6">
+        <v>158305</v>
+      </c>
+      <c r="X173" s="6">
+        <v>156500</v>
+      </c>
+      <c r="Y173" s="6">
+        <v>153831</v>
+      </c>
       <c r="Z173" s="4"/>
     </row>
     <row r="174" ht="14.5" customHeight="1">
@@ -10651,790 +10870,78 @@
         <v>26</v>
       </c>
       <c r="B175" s="6">
-        <v>2167274</v>
+        <v>67010</v>
       </c>
       <c r="C175" s="6">
-        <v>2141025</v>
+        <v>61613</v>
       </c>
       <c r="D175" s="6">
-        <v>2120467</v>
+        <v>57534</v>
       </c>
       <c r="E175" s="6">
-        <v>2085743</v>
+        <v>55309</v>
       </c>
       <c r="F175" s="6">
-        <v>2067342</v>
+        <v>53137</v>
       </c>
       <c r="G175" s="6">
-        <v>2048582</v>
+        <v>51933</v>
       </c>
       <c r="H175" s="6">
-        <v>2028377</v>
+        <v>51815</v>
       </c>
       <c r="I175" s="6">
-        <v>2006536</v>
+        <v>52391</v>
       </c>
       <c r="J175" s="6">
-        <v>1988580</v>
+        <v>52913</v>
       </c>
       <c r="K175" s="6">
-        <v>1977392</v>
+        <v>52825</v>
       </c>
       <c r="L175" s="6">
-        <v>1969602</v>
+        <v>52138</v>
       </c>
       <c r="M175" s="6">
-        <v>1965178</v>
+        <v>51179</v>
       </c>
       <c r="N175" s="6">
-        <v>1953545</v>
+        <v>50346</v>
       </c>
       <c r="O175" s="6">
-        <v>1950483</v>
+        <v>50988</v>
       </c>
       <c r="P175" s="6">
-        <v>1947263</v>
+        <v>50780</v>
       </c>
       <c r="Q175" s="6">
-        <v>1938516</v>
+        <v>50555</v>
       </c>
       <c r="R175" s="6">
-        <v>1933308</v>
+        <v>50540</v>
       </c>
       <c r="S175" s="6">
-        <v>1929008</v>
+        <v>50157</v>
       </c>
       <c r="T175" s="6">
-        <v>1923116</v>
+        <v>49822</v>
       </c>
       <c r="U175" s="6">
-        <v>1913037</v>
+        <v>49348</v>
       </c>
       <c r="V175" s="6">
-        <v>1902718</v>
+        <v>49663</v>
       </c>
       <c r="W175" s="6">
-        <v>1895868</v>
+        <v>50288</v>
       </c>
       <c r="X175" s="6">
-        <v>1877844</v>
+        <v>49527</v>
       </c>
       <c r="Y175" s="6">
-        <v>1863011</v>
+        <v>50040</v>
       </c>
       <c r="Z175" s="4"/>
-    </row>
-    <row r="176" ht="14.5" customHeight="1">
-      <c r="A176" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="B176" s="5"/>
-      <c r="C176" s="5"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="5"/>
-      <c r="F176" s="5"/>
-      <c r="G176" s="5"/>
-      <c r="H176" s="5"/>
-      <c r="I176" s="5"/>
-      <c r="J176" s="5"/>
-      <c r="K176" s="5"/>
-      <c r="L176" s="5"/>
-      <c r="M176" s="5"/>
-      <c r="N176" s="5"/>
-      <c r="O176" s="5"/>
-      <c r="P176" s="5"/>
-      <c r="Q176" s="5"/>
-      <c r="R176" s="5"/>
-      <c r="S176" s="5"/>
-      <c r="T176" s="5"/>
-      <c r="U176" s="5"/>
-      <c r="V176" s="5"/>
-      <c r="W176" s="5"/>
-      <c r="X176" s="5"/>
-      <c r="Y176" s="5"/>
-      <c r="Z176" s="4"/>
-    </row>
-    <row r="177" ht="38.5" customHeight="1">
-      <c r="A177" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B177" s="6">
-        <v>1493881</v>
-      </c>
-      <c r="C177" s="6">
-        <v>1473876</v>
-      </c>
-      <c r="D177" s="6">
-        <v>1459908</v>
-      </c>
-      <c r="E177" s="6">
-        <v>1446177</v>
-      </c>
-      <c r="F177" s="6">
-        <v>1434242</v>
-      </c>
-      <c r="G177" s="6">
-        <v>1416224</v>
-      </c>
-      <c r="H177" s="6">
-        <v>1396800</v>
-      </c>
-      <c r="I177" s="6">
-        <v>1376260</v>
-      </c>
-      <c r="J177" s="6">
-        <v>1359894</v>
-      </c>
-      <c r="K177" s="6">
-        <v>1354848</v>
-      </c>
-      <c r="L177" s="6">
-        <v>1351123</v>
-      </c>
-      <c r="M177" s="6">
-        <v>1349230</v>
-      </c>
-      <c r="N177" s="6">
-        <v>1342887</v>
-      </c>
-      <c r="O177" s="6">
-        <v>1342475</v>
-      </c>
-      <c r="P177" s="6">
-        <v>1342083</v>
-      </c>
-      <c r="Q177" s="6">
-        <v>1339912</v>
-      </c>
-      <c r="R177" s="6">
-        <v>1338305</v>
-      </c>
-      <c r="S177" s="6">
-        <v>1334552</v>
-      </c>
-      <c r="T177" s="6">
-        <v>1333294</v>
-      </c>
-      <c r="U177" s="6">
-        <v>1328302</v>
-      </c>
-      <c r="V177" s="6">
-        <v>1321473</v>
-      </c>
-      <c r="W177" s="6">
-        <v>1315643</v>
-      </c>
-      <c r="X177" s="6">
-        <v>1301127</v>
-      </c>
-      <c r="Y177" s="6">
-        <v>1298978</v>
-      </c>
-      <c r="Z177" s="4"/>
-    </row>
-    <row r="178" ht="14.5" customHeight="1">
-      <c r="A178" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="B178" s="5"/>
-      <c r="C178" s="5"/>
-      <c r="D178" s="5"/>
-      <c r="E178" s="5"/>
-      <c r="F178" s="5"/>
-      <c r="G178" s="5"/>
-      <c r="H178" s="5"/>
-      <c r="I178" s="5"/>
-      <c r="J178" s="5"/>
-      <c r="K178" s="5"/>
-      <c r="L178" s="5"/>
-      <c r="M178" s="5"/>
-      <c r="N178" s="5"/>
-      <c r="O178" s="5"/>
-      <c r="P178" s="5"/>
-      <c r="Q178" s="5"/>
-      <c r="R178" s="5"/>
-      <c r="S178" s="5"/>
-      <c r="T178" s="5"/>
-      <c r="U178" s="5"/>
-      <c r="V178" s="5"/>
-      <c r="W178" s="5"/>
-      <c r="X178" s="5"/>
-      <c r="Y178" s="5"/>
-      <c r="Z178" s="4"/>
-    </row>
-    <row r="179" ht="38.5" customHeight="1">
-      <c r="A179" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B179" s="6">
-        <v>949526</v>
-      </c>
-      <c r="C179" s="6">
-        <v>935607</v>
-      </c>
-      <c r="D179" s="6">
-        <v>923055</v>
-      </c>
-      <c r="E179" s="6">
-        <v>911381</v>
-      </c>
-      <c r="F179" s="6">
-        <v>901044</v>
-      </c>
-      <c r="G179" s="6">
-        <v>887781</v>
-      </c>
-      <c r="H179" s="6">
-        <v>874018</v>
-      </c>
-      <c r="I179" s="6">
-        <v>861056</v>
-      </c>
-      <c r="J179" s="6">
-        <v>850502</v>
-      </c>
-      <c r="K179" s="6">
-        <v>844290</v>
-      </c>
-      <c r="L179" s="6">
-        <v>838869</v>
-      </c>
-      <c r="M179" s="6">
-        <v>834905</v>
-      </c>
-      <c r="N179" s="6">
-        <v>828660</v>
-      </c>
-      <c r="O179" s="6">
-        <v>821573</v>
-      </c>
-      <c r="P179" s="6">
-        <v>816910</v>
-      </c>
-      <c r="Q179" s="6">
-        <v>811274</v>
-      </c>
-      <c r="R179" s="6">
-        <v>809873</v>
-      </c>
-      <c r="S179" s="6">
-        <v>805689</v>
-      </c>
-      <c r="T179" s="6">
-        <v>801752</v>
-      </c>
-      <c r="U179" s="6">
-        <v>798424</v>
-      </c>
-      <c r="V179" s="6">
-        <v>793194</v>
-      </c>
-      <c r="W179" s="6">
-        <v>790044</v>
-      </c>
-      <c r="X179" s="6">
-        <v>781846</v>
-      </c>
-      <c r="Y179" s="6">
-        <v>772525</v>
-      </c>
-      <c r="Z179" s="4"/>
-    </row>
-    <row r="180" ht="14.5" customHeight="1">
-      <c r="A180" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="B180" s="5"/>
-      <c r="C180" s="5"/>
-      <c r="D180" s="5"/>
-      <c r="E180" s="5"/>
-      <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
-      <c r="H180" s="5"/>
-      <c r="I180" s="5"/>
-      <c r="J180" s="5"/>
-      <c r="K180" s="5"/>
-      <c r="L180" s="5"/>
-      <c r="M180" s="5"/>
-      <c r="N180" s="5"/>
-      <c r="O180" s="5"/>
-      <c r="P180" s="5"/>
-      <c r="Q180" s="5"/>
-      <c r="R180" s="5"/>
-      <c r="S180" s="5"/>
-      <c r="T180" s="5"/>
-      <c r="U180" s="5"/>
-      <c r="V180" s="5"/>
-      <c r="W180" s="5"/>
-      <c r="X180" s="5"/>
-      <c r="Y180" s="5"/>
-      <c r="Z180" s="4"/>
-    </row>
-    <row r="181" ht="38.5" customHeight="1">
-      <c r="A181" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B181" s="6">
-        <v>211696</v>
-      </c>
-      <c r="C181" s="6">
-        <v>201974</v>
-      </c>
-      <c r="D181" s="6">
-        <v>193945</v>
-      </c>
-      <c r="E181" s="6">
-        <v>187218</v>
-      </c>
-      <c r="F181" s="6">
-        <v>181832</v>
-      </c>
-      <c r="G181" s="6">
-        <v>178069</v>
-      </c>
-      <c r="H181" s="6">
-        <v>173937</v>
-      </c>
-      <c r="I181" s="6">
-        <v>170397</v>
-      </c>
-      <c r="J181" s="6">
-        <v>166902</v>
-      </c>
-      <c r="K181" s="6">
-        <v>163989</v>
-      </c>
-      <c r="L181" s="6">
-        <v>160940</v>
-      </c>
-      <c r="M181" s="6">
-        <v>159002</v>
-      </c>
-      <c r="N181" s="6">
-        <v>156534</v>
-      </c>
-      <c r="O181" s="6">
-        <v>154485</v>
-      </c>
-      <c r="P181" s="6">
-        <v>152358</v>
-      </c>
-      <c r="Q181" s="6">
-        <v>150312</v>
-      </c>
-      <c r="R181" s="6">
-        <v>148071</v>
-      </c>
-      <c r="S181" s="6">
-        <v>146345</v>
-      </c>
-      <c r="T181" s="6">
-        <v>145570</v>
-      </c>
-      <c r="U181" s="6">
-        <v>144091</v>
-      </c>
-      <c r="V181" s="6">
-        <v>141234</v>
-      </c>
-      <c r="W181" s="6">
-        <v>140149</v>
-      </c>
-      <c r="X181" s="6">
-        <v>139034</v>
-      </c>
-      <c r="Y181" s="6">
-        <v>137767</v>
-      </c>
-      <c r="Z181" s="4"/>
-    </row>
-    <row r="182" ht="14.5" customHeight="1">
-      <c r="A182" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
-      <c r="D182" s="5"/>
-      <c r="E182" s="5"/>
-      <c r="F182" s="5"/>
-      <c r="G182" s="5"/>
-      <c r="H182" s="5"/>
-      <c r="I182" s="5"/>
-      <c r="J182" s="5"/>
-      <c r="K182" s="5"/>
-      <c r="L182" s="5"/>
-      <c r="M182" s="5"/>
-      <c r="N182" s="5"/>
-      <c r="O182" s="5"/>
-      <c r="P182" s="5"/>
-      <c r="Q182" s="5"/>
-      <c r="R182" s="5"/>
-      <c r="S182" s="5"/>
-      <c r="T182" s="5"/>
-      <c r="U182" s="5"/>
-      <c r="V182" s="5"/>
-      <c r="W182" s="5"/>
-      <c r="X182" s="5"/>
-      <c r="Y182" s="5"/>
-      <c r="Z182" s="4"/>
-    </row>
-    <row r="183" ht="38.5" customHeight="1">
-      <c r="A183" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B183" s="6">
-        <v>581305</v>
-      </c>
-      <c r="C183" s="6">
-        <v>569234</v>
-      </c>
-      <c r="D183" s="6">
-        <v>560049</v>
-      </c>
-      <c r="E183" s="6">
-        <v>552155</v>
-      </c>
-      <c r="F183" s="6">
-        <v>545008</v>
-      </c>
-      <c r="G183" s="6">
-        <v>536783</v>
-      </c>
-      <c r="H183" s="6">
-        <v>529813</v>
-      </c>
-      <c r="I183" s="6">
-        <v>521121</v>
-      </c>
-      <c r="J183" s="6">
-        <v>513452</v>
-      </c>
-      <c r="K183" s="6">
-        <v>509364</v>
-      </c>
-      <c r="L183" s="6">
-        <v>504896</v>
-      </c>
-      <c r="M183" s="6">
-        <v>501279</v>
-      </c>
-      <c r="N183" s="6">
-        <v>496739</v>
-      </c>
-      <c r="O183" s="6">
-        <v>495402</v>
-      </c>
-      <c r="P183" s="6">
-        <v>493302</v>
-      </c>
-      <c r="Q183" s="6">
-        <v>491027</v>
-      </c>
-      <c r="R183" s="6">
-        <v>488391</v>
-      </c>
-      <c r="S183" s="6">
-        <v>487293</v>
-      </c>
-      <c r="T183" s="6">
-        <v>487344</v>
-      </c>
-      <c r="U183" s="6">
-        <v>490181</v>
-      </c>
-      <c r="V183" s="6">
-        <v>489638</v>
-      </c>
-      <c r="W183" s="6">
-        <v>488257</v>
-      </c>
-      <c r="X183" s="6">
-        <v>485621</v>
-      </c>
-      <c r="Y183" s="6">
-        <v>484177</v>
-      </c>
-      <c r="Z183" s="4"/>
-    </row>
-    <row r="184" ht="14.5" customHeight="1">
-      <c r="A184" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="B184" s="5"/>
-      <c r="C184" s="5"/>
-      <c r="D184" s="5"/>
-      <c r="E184" s="5"/>
-      <c r="F184" s="5"/>
-      <c r="G184" s="5"/>
-      <c r="H184" s="5"/>
-      <c r="I184" s="5"/>
-      <c r="J184" s="5"/>
-      <c r="K184" s="5"/>
-      <c r="L184" s="5"/>
-      <c r="M184" s="5"/>
-      <c r="N184" s="5"/>
-      <c r="O184" s="5"/>
-      <c r="P184" s="5"/>
-      <c r="Q184" s="5"/>
-      <c r="R184" s="5"/>
-      <c r="S184" s="5"/>
-      <c r="T184" s="5"/>
-      <c r="U184" s="5"/>
-      <c r="V184" s="5"/>
-      <c r="W184" s="5"/>
-      <c r="X184" s="5"/>
-      <c r="Y184" s="5"/>
-      <c r="Z184" s="4"/>
-    </row>
-    <row r="185" ht="38.5" customHeight="1">
-      <c r="A185" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B185" s="6">
-        <v>199172</v>
-      </c>
-      <c r="C185" s="6">
-        <v>195135</v>
-      </c>
-      <c r="D185" s="6">
-        <v>193198</v>
-      </c>
-      <c r="E185" s="6">
-        <v>191899</v>
-      </c>
-      <c r="F185" s="6">
-        <v>190585</v>
-      </c>
-      <c r="G185" s="6">
-        <v>188412</v>
-      </c>
-      <c r="H185" s="6">
-        <v>185763</v>
-      </c>
-      <c r="I185" s="6">
-        <v>181653</v>
-      </c>
-      <c r="J185" s="6">
-        <v>179405</v>
-      </c>
-      <c r="K185" s="6">
-        <v>178711</v>
-      </c>
-      <c r="L185" s="6">
-        <v>178148</v>
-      </c>
-      <c r="M185" s="6">
-        <v>177500</v>
-      </c>
-      <c r="N185" s="6">
-        <v>176304</v>
-      </c>
-      <c r="O185" s="6">
-        <v>174412</v>
-      </c>
-      <c r="P185" s="6">
-        <v>172671</v>
-      </c>
-      <c r="Q185" s="6">
-        <v>170377</v>
-      </c>
-      <c r="R185" s="6">
-        <v>168368</v>
-      </c>
-      <c r="S185" s="6">
-        <v>166120</v>
-      </c>
-      <c r="T185" s="6">
-        <v>164217</v>
-      </c>
-      <c r="U185" s="6">
-        <v>162014</v>
-      </c>
-      <c r="V185" s="6">
-        <v>159913</v>
-      </c>
-      <c r="W185" s="6">
-        <v>158305</v>
-      </c>
-      <c r="X185" s="6">
-        <v>156500</v>
-      </c>
-      <c r="Y185" s="6">
-        <v>153831</v>
-      </c>
-      <c r="Z185" s="4"/>
-    </row>
-    <row r="186" ht="14.5" customHeight="1">
-      <c r="A186" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="B186" s="5"/>
-      <c r="C186" s="5"/>
-      <c r="D186" s="5"/>
-      <c r="E186" s="5"/>
-      <c r="F186" s="5"/>
-      <c r="G186" s="5"/>
-      <c r="H186" s="5"/>
-      <c r="I186" s="5"/>
-      <c r="J186" s="5"/>
-      <c r="K186" s="5"/>
-      <c r="L186" s="5"/>
-      <c r="M186" s="5"/>
-      <c r="N186" s="5"/>
-      <c r="O186" s="5"/>
-      <c r="P186" s="5"/>
-      <c r="Q186" s="5"/>
-      <c r="R186" s="5"/>
-      <c r="S186" s="5"/>
-      <c r="T186" s="5"/>
-      <c r="U186" s="5"/>
-      <c r="V186" s="5"/>
-      <c r="W186" s="5"/>
-      <c r="X186" s="5"/>
-      <c r="Y186" s="5"/>
-      <c r="Z186" s="4"/>
-    </row>
-    <row r="187" ht="38.5" customHeight="1">
-      <c r="A187" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B187" s="6">
-        <v>67010</v>
-      </c>
-      <c r="C187" s="6">
-        <v>61613</v>
-      </c>
-      <c r="D187" s="6">
-        <v>57534</v>
-      </c>
-      <c r="E187" s="6">
-        <v>55309</v>
-      </c>
-      <c r="F187" s="6">
-        <v>53137</v>
-      </c>
-      <c r="G187" s="6">
-        <v>51933</v>
-      </c>
-      <c r="H187" s="6">
-        <v>51815</v>
-      </c>
-      <c r="I187" s="6">
-        <v>52391</v>
-      </c>
-      <c r="J187" s="6">
-        <v>52913</v>
-      </c>
-      <c r="K187" s="6">
-        <v>52825</v>
-      </c>
-      <c r="L187" s="6">
-        <v>52138</v>
-      </c>
-      <c r="M187" s="6">
-        <v>51179</v>
-      </c>
-      <c r="N187" s="6">
-        <v>50346</v>
-      </c>
-      <c r="O187" s="6">
-        <v>50988</v>
-      </c>
-      <c r="P187" s="6">
-        <v>50780</v>
-      </c>
-      <c r="Q187" s="6">
-        <v>50555</v>
-      </c>
-      <c r="R187" s="6">
-        <v>50540</v>
-      </c>
-      <c r="S187" s="6">
-        <v>50157</v>
-      </c>
-      <c r="T187" s="6">
-        <v>49822</v>
-      </c>
-      <c r="U187" s="6">
-        <v>49348</v>
-      </c>
-      <c r="V187" s="6">
-        <v>49663</v>
-      </c>
-      <c r="W187" s="6">
-        <v>50288</v>
-      </c>
-      <c r="X187" s="6">
-        <v>49527</v>
-      </c>
-      <c r="Y187" s="6">
-        <v>50040</v>
-      </c>
-      <c r="Z187" s="4"/>
-    </row>
-    <row r="188" ht="14.5" customHeight="1">
-      <c r="A188" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="B188" s="5"/>
-      <c r="C188" s="5"/>
-      <c r="D188" s="5"/>
-      <c r="E188" s="5"/>
-      <c r="F188" s="5"/>
-      <c r="G188" s="5"/>
-      <c r="H188" s="5"/>
-      <c r="I188" s="5"/>
-      <c r="J188" s="5"/>
-      <c r="K188" s="5"/>
-      <c r="L188" s="5"/>
-      <c r="M188" s="5"/>
-      <c r="N188" s="5"/>
-      <c r="O188" s="5"/>
-      <c r="P188" s="5"/>
-      <c r="Q188" s="5"/>
-      <c r="R188" s="5"/>
-      <c r="S188" s="5"/>
-      <c r="T188" s="5"/>
-      <c r="U188" s="5"/>
-      <c r="V188" s="5"/>
-      <c r="W188" s="5"/>
-      <c r="X188" s="5"/>
-      <c r="Y188" s="5"/>
-      <c r="Z188" s="4"/>
-    </row>
-    <row r="189" ht="38.5" customHeight="1">
-      <c r="A189" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B189" s="5"/>
-      <c r="C189" s="5"/>
-      <c r="D189" s="5"/>
-      <c r="E189" s="5"/>
-      <c r="F189" s="5"/>
-      <c r="G189" s="5"/>
-      <c r="H189" s="5"/>
-      <c r="I189" s="5"/>
-      <c r="J189" s="5"/>
-      <c r="K189" s="5"/>
-      <c r="L189" s="5"/>
-      <c r="M189" s="5"/>
-      <c r="N189" s="5"/>
-      <c r="O189" s="5"/>
-      <c r="P189" s="5"/>
-      <c r="Q189" s="5"/>
-      <c r="R189" s="6">
-        <v>2294888</v>
-      </c>
-      <c r="S189" s="6">
-        <v>2323369</v>
-      </c>
-      <c r="T189" s="5"/>
-      <c r="U189" s="5"/>
-      <c r="V189" s="5"/>
-      <c r="W189" s="5"/>
-      <c r="X189" s="5"/>
-      <c r="Y189" s="5"/>
-      <c r="Z189" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>